<commit_message>
use expriment type indices for plots instead of drop indices, read drop indices and experiment name from xls file
</commit_message>
<xml_diff>
--- a/3D networks data.xlsx
+++ b/3D networks data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niv\Documents\MATLAB\Matlab code GUI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niv\Documents\MATLAB\Maya code GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
-  <si>
-    <t>Niv Experiment</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -207,6 +204,12 @@
   </si>
   <si>
     <t>W:\phkinnerets\storage\analysis\Niv\las17\2018_10_03\mix1 rambam10 + 5uM las17\Capture 8</t>
+  </si>
+  <si>
+    <t>5uM Las17</t>
+  </si>
+  <si>
+    <t>5uM Las27</t>
   </si>
 </sst>
 </file>
@@ -548,7 +551,7 @@
   <dimension ref="A1:BF6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,178 +564,178 @@
   <sheetData>
     <row r="1" spans="1:58" s="4" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="BB1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="BC1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="BD1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="BA1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="BB1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="BC1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="BF1" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.25">
@@ -740,13 +743,13 @@
         <v>43376</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -772,13 +775,13 @@
         <v>43376</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.25">
@@ -786,13 +789,13 @@
         <v>43376</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.25">
@@ -800,13 +803,13 @@
         <v>43376</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.25">
@@ -814,13 +817,13 @@
         <v>43376</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
determine color automatically, fix bug with excel indices
</commit_message>
<xml_diff>
--- a/3D networks data.xlsx
+++ b/3D networks data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
   <si>
     <t>Date</t>
   </si>
@@ -210,6 +210,33 @@
   </si>
   <si>
     <t>5uM Las27</t>
+  </si>
+  <si>
+    <t>Rambam 12</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam12 extract\test extract\2019_02_07\Capture 1\</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam12 extract\test extract\2019_02_07\Capture 2\</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam12 extract\test extract\2019_02_07\Capture 3\</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam12 extract\test extract\2019_02_07\Capture 4\</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam12 extract\test extract\2019_02_07\Capture 5\</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam12 extract\test extract\2019_02_07\Capture 6\</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam12 extract\test extract\2019_02_07\Capture 7\</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam12 extract\test extract\2019_02_07\Capture 8\</t>
   </si>
 </sst>
 </file>
@@ -548,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF6"/>
+  <dimension ref="A1:BF15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,6 +853,118 @@
         <v>58</v>
       </c>
     </row>
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>43503</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="1">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>43503</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="1">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>43503</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="1">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>43503</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="1">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>43503</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="1">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>43503</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="1">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>43503</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="1">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>43503</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="1">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add my recent experiments
</commit_message>
<xml_diff>
--- a/3D networks data.xlsx
+++ b/3D networks data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20352"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niv\Documents\MATLAB\Maya code GUI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niv\Documents\MATLAB\Maya code GUI - Niv\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC25D8F-EAD4-4147-BFF0-60D48D2A34B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19185" windowHeight="7035"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19185" windowHeight="7035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="171">
   <si>
     <t>Date</t>
   </si>
@@ -191,21 +192,6 @@
     <t xml:space="preserve">assembly rate </t>
   </si>
   <si>
-    <t>W:\phkinnerets\storage\analysis\Niv\las17\2018_10_03\mix1 rambam10 + 5uM las17\Capture 3</t>
-  </si>
-  <si>
-    <t>W:\phkinnerets\storage\analysis\Niv\las17\2018_10_03\mix1 rambam10 + 5uM las17\Capture 5</t>
-  </si>
-  <si>
-    <t>W:\phkinnerets\storage\analysis\Niv\las17\2018_10_03\mix1 rambam10 + 5uM las17\Capture 6</t>
-  </si>
-  <si>
-    <t>W:\phkinnerets\storage\analysis\Niv\las17\2018_10_03\mix1 rambam10 + 5uM las17\Capture 9</t>
-  </si>
-  <si>
-    <t>W:\phkinnerets\storage\analysis\Niv\las17\2018_10_03\mix1 rambam10 + 5uM las17\Capture 8</t>
-  </si>
-  <si>
     <t>5uM Las17</t>
   </si>
   <si>
@@ -237,12 +223,327 @@
   </si>
   <si>
     <t>W:\phkinnerets\storage\analysis\Niv\rambam12 extract\test extract\2019_02_07\Capture 8\</t>
+  </si>
+  <si>
+    <t>80% extract xb</t>
+  </si>
+  <si>
+    <t>\Maya Analysis after GRC\Data Analysis\2017_08_08\80%extract xb\mix1 14_05\Capture 9\</t>
+  </si>
+  <si>
+    <t>\Maya Analysis after GRC\Data Analysis\2017_08_08\80%extract xb\mix1 15_00\Capture 1\</t>
+  </si>
+  <si>
+    <t>\Maya Analysis after GRC\Data Analysis\2017_08_08\80%extract xb\mix1 15_00\Capture 2\</t>
+  </si>
+  <si>
+    <t>\Maya Analysis after GRC\Data Analysis\2017_08_08\80%extract xb\mix1 15_00\Capture 4\</t>
+  </si>
+  <si>
+    <t>\Maya Analysis after GRC\Data Analysis\2017_08_08\80%extract xb\mix1 15_00\Capture 5\</t>
+  </si>
+  <si>
+    <t>\Maya Analysis after GRC\Data Analysis\2017_08_15\80%extract xb\Mix1 11_00\Capture 1\</t>
+  </si>
+  <si>
+    <t>\Maya Analysis after GRC\Data Analysis\2017_08_15\80%extract xb\Mix1 11_00\Capture 6\</t>
+  </si>
+  <si>
+    <t>\Maya Analysis after GRC\Data Analysis\2017_08_15\80%extract xb\Mix1 11_00\Capture 7\</t>
+  </si>
+  <si>
+    <t>\Maya Analysis after GRC\Data Analysis\2017_08_15\80%extract xb\Mix1 11_40\Capture 4\</t>
+  </si>
+  <si>
+    <t>\Maya Analysis after GRC\Data Analysis\2017_08_15\80%extract xb\Mix1 11_40\Capture 6\</t>
+  </si>
+  <si>
+    <t>\Maya Analysis after GRC\Data Analysis\2017_08_15\80%extract xb\Mix1 11_40\Capture 8\</t>
+  </si>
+  <si>
+    <t>\Maya Analysis after GRC\Data Analysis\2017_08_15\80%extract xb\Mix1 12_20\Capture 3\</t>
+  </si>
+  <si>
+    <t>\Maya Analysis after GRC\Data Analysis\2017_08_15\80%extract xb\Mix1 12_20\Capture 5\</t>
+  </si>
+  <si>
+    <t>Rambam5 + 0.5uM cytochalasin D</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\cytochalasin D\2019_11_03\mix1 sample1\Capture 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\cytochalasin D\2019_11_03\mix1 sample1\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\cytochalasin D\2019_11_03\mix1 sample1\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\cytochalasin D\2019_11_03\mix1 sample1\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\cytochalasin D\2019_11_03\mix1 sample1\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\cytochalasin D\2019_11_03\mix1 sample1\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\cytochalasin D\2019_11_03\mix1 sample2\Capture 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\cytochalasin D\2019_11_03\mix1 sample2\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\cytochalasin D\2019_11_03\mix1 sample2\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\cytochalasin D\2019_11_03\mix1 sample2\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\cytochalasin D\2019_11_03\mix1 sample2\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\cytochalasin D\2019_11_03\mix1 sample2\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\las17 and cortices\2018_10_03\mix1 rambam10 + 5uM las17\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\las17 and cortices\2018_10_03\mix1 rambam10 + 5uM las17\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\las17 and cortices\2018_10_03\mix1 rambam10 + 5uM las17\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\las17 and cortices\2018_10_03\mix1 rambam10 + 5uM las17\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\las17 and cortices\2018_10_03\mix1 rambam10 + 5uM las17\Capture 9</t>
+  </si>
+  <si>
+    <t>\Maya Analysis after GRC\Data Analysis\2017_12_21\Mix2 14_05\Capture 14\</t>
+  </si>
+  <si>
+    <t>\Maya Analysis after GRC\Data Analysis\2017_12_21\mix2 14_40\Capture 2\</t>
+  </si>
+  <si>
+    <t>\Maya Analysis after GRC\Data Analysis\2017_12_21\mix2 14_40\Capture 5\</t>
+  </si>
+  <si>
+    <t>\Maya Analysis after GRC\Data Analysis\2017_12_21\mix2 14_40\Capture 8\</t>
+  </si>
+  <si>
+    <t>\Maya Analysis after GRC\Data Analysis\2017_12_21\mix2 14_40\Capture 10\</t>
+  </si>
+  <si>
+    <t>\Maya Analysis after GRC\Data Analysis\2017_12_21\mix2 14_40\Capture 14\</t>
+  </si>
+  <si>
+    <t>problem in analysis</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\cytochalasin D\2019_11_03\mix1 sample2\Capture 5</t>
+  </si>
+  <si>
+    <t>couldn't analyse</t>
+  </si>
+  <si>
+    <t>significantly slower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rambam 10 </t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\2018_06_20\Capture 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\2018_06_20\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\2018_06_20\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\2018_12_03\Capture 1</t>
+  </si>
+  <si>
+    <t>20/06/2018</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\2018_12_03\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\2018_12_03\Capture 13</t>
+  </si>
+  <si>
+    <t>Rambam10 I-phase</t>
+  </si>
+  <si>
+    <t>Rambam10 I-phase no CH</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\I-phase\2019_11_11\Ca only\Capture 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\I-phase\2019_11_11\Ca only\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\I-phase\2019_11_11\Ca only\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\I-phase\2019_11_11\Ca only\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\I-phase\2019_11_11\Ca only\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\I-phase\2019_11_11\Ca only\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\I-phase\2019_11_11\Ca only\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\I-phase\2019_11_11\Ca only\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\I-phase\2019_11_11\Ca only\Capture 9</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\I-phase\2019_11_11\Ca only\Capture 10</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\I-phase\2019_11_11\Ca only\Capture 4 - 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\I-phase\2019_11_11\Ca only\Capture 3 - 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\I-phase\2019_11_11\Ca only\Capture 5 - 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\I-phase\2019_11_11\Ca only\Capture 6 - 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\I-phase\2019_11_11\Ca only\Capture 7 - 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\I-phase\2019_11_11\Ca only\Capture 11</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\I-phase\2019_11_11\Ca only\Capture 12</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_11_20\30um\Capture 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_11_20\30um\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_11_20\30um\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_11_20\30um\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_11_20\30um\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_11_20\30um\Capture 6</t>
+  </si>
+  <si>
+    <t>20/11/2019</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_11_11\Ca+CH\Capture 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_11_11\Ca+CH\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_11_11\Ca+CH\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_11_11\Ca+CH\Capture 9</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_11_11\Ca+CH\Capture 10</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_11_11\Ca+CH\Capture 11</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_11_11\Ca+CH\Capture 12</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_11_11\Ca+CH\Capture 13</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_11_11\Ca+CH\Capture 14</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_11_11\Ca+CH\Capture 15</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_11_11\Ca+CH\Capture 16</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_11_11\Ca+CH\Capture 17</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\60%\2019_11_20\30um\Capture 1</t>
+  </si>
+  <si>
+    <t>Rambam 10 60%</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\60%\2019_11_20\30um\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\60%\2019_11_20\30um\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\60%\2019_11_20\30um\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\60%\2019_11_20\30um\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\60%\2019_11_20\30um\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\60%\2019_11_20\30um\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\60%\2019_11_20\30um\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\40%\2019_11_20\30um\Capture 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\40%\2019_11_20\30um\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\40%\2019_11_20\30um\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\40%\2019_11_20\30um\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\40%\2019_11_20\30um\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\40%\2019_11_20\30um\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\40%\2019_11_20\30um\Capture 7</t>
+  </si>
+  <si>
+    <t>Rambam 10 40%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -260,12 +561,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -280,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -295,6 +602,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,11 +886,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BF113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,13 +1082,13 @@
         <v>43376</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -802,13 +1114,13 @@
         <v>43376</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C3" s="1">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:58" x14ac:dyDescent="0.25">
@@ -816,13 +1128,13 @@
         <v>43376</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:58" x14ac:dyDescent="0.25">
@@ -830,13 +1142,13 @@
         <v>43376</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:58" x14ac:dyDescent="0.25">
@@ -844,13 +1156,13 @@
         <v>43376</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C6" s="1">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:58" x14ac:dyDescent="0.25">
@@ -858,13 +1170,13 @@
         <v>43503</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1">
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:58" x14ac:dyDescent="0.25">
@@ -872,13 +1184,13 @@
         <v>43503</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1">
         <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:58" x14ac:dyDescent="0.25">
@@ -886,13 +1198,13 @@
         <v>43503</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C10" s="1">
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:58" x14ac:dyDescent="0.25">
@@ -900,13 +1212,13 @@
         <v>43503</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C11" s="1">
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:58" x14ac:dyDescent="0.25">
@@ -914,13 +1226,13 @@
         <v>43503</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1">
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:58" x14ac:dyDescent="0.25">
@@ -928,13 +1240,13 @@
         <v>43503</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C13" s="1">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:58" x14ac:dyDescent="0.25">
@@ -942,13 +1254,13 @@
         <v>43503</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C14" s="1">
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:58" x14ac:dyDescent="0.25">
@@ -956,13 +1268,1387 @@
         <v>43503</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C15" s="1">
         <v>12</v>
       </c>
       <c r="D15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>20170808</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="1">
+        <v>64</v>
+      </c>
+      <c r="D17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>20170808</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="1">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>20170808</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="1">
+        <v>64</v>
+      </c>
+      <c r="D19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20170808</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="1">
+        <v>64</v>
+      </c>
+      <c r="D20" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20170808</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="1">
+        <v>64</v>
+      </c>
+      <c r="D21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20170815</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="1">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>20170815</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="1">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>20170815</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="1">
+        <v>37</v>
+      </c>
+      <c r="D25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>20170815</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="1">
+        <v>37</v>
+      </c>
+      <c r="D26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>20170815</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="1">
+        <v>37</v>
+      </c>
+      <c r="D27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>20170815</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="1">
+        <v>37</v>
+      </c>
+      <c r="D28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>20170815</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="1">
+        <v>37</v>
+      </c>
+      <c r="D29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>20170815</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="1">
+        <v>37</v>
+      </c>
+      <c r="D30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>20171221</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="1">
+        <v>37</v>
+      </c>
+      <c r="D31" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>20171221</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="1">
+        <v>37</v>
+      </c>
+      <c r="D32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>20171221</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="1">
+        <v>37</v>
+      </c>
+      <c r="D33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>20171221</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="1">
+        <v>37</v>
+      </c>
+      <c r="D34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>20171221</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="1">
+        <v>37</v>
+      </c>
+      <c r="D35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>20171221</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="1">
+        <v>37</v>
+      </c>
+      <c r="D36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>43535</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2001</v>
+      </c>
+      <c r="D38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>43535</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2001</v>
+      </c>
+      <c r="D39" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>43535</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2001</v>
+      </c>
+      <c r="D40" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>43535</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" s="1">
+        <v>2001</v>
+      </c>
+      <c r="D41" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>43535</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2001</v>
+      </c>
+      <c r="D42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <v>43535</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="1">
+        <v>2001</v>
+      </c>
+      <c r="D43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="8">
+        <v>43535</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="7">
+        <v>-2001</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="8">
+        <v>43535</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="7">
+        <v>-2001</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="8">
+        <v>43535</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="7">
+        <v>-2001</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="Q46" s="7"/>
+      <c r="R46" s="7"/>
+      <c r="U46" s="7"/>
+      <c r="V46" s="7"/>
+      <c r="W46" s="7"/>
+      <c r="X46" s="7"/>
+      <c r="Y46" s="7"/>
+      <c r="Z46" s="7"/>
+      <c r="AA46" s="7"/>
+      <c r="AB46" s="7"/>
+      <c r="AC46" s="7"/>
+      <c r="AD46" s="7"/>
+      <c r="AE46" s="7"/>
+      <c r="AF46" s="7"/>
+      <c r="AG46" s="7"/>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <v>43535</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="1">
+        <v>2001</v>
+      </c>
+      <c r="D47" t="s">
+        <v>90</v>
+      </c>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="U47" s="1"/>
+      <c r="V47" s="1"/>
+      <c r="W47" s="1"/>
+      <c r="X47" s="1"/>
+      <c r="Y47" s="1"/>
+      <c r="Z47" s="1"/>
+      <c r="AA47" s="1"/>
+      <c r="AB47" s="1"/>
+      <c r="AC47" s="1"/>
+      <c r="AD47" s="1"/>
+      <c r="AE47" s="1"/>
+      <c r="AF47" s="1"/>
+      <c r="AG47" s="1"/>
+    </row>
+    <row r="48" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8">
+        <v>43535</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" s="7">
+        <v>-2001</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="7"/>
+      <c r="Q48" s="7"/>
+      <c r="R48" s="7"/>
+      <c r="U48" s="7"/>
+      <c r="V48" s="7"/>
+      <c r="W48" s="7"/>
+      <c r="X48" s="7"/>
+      <c r="Y48" s="7"/>
+      <c r="Z48" s="7"/>
+      <c r="AA48" s="7"/>
+      <c r="AB48" s="7"/>
+      <c r="AC48" s="7"/>
+      <c r="AD48" s="7"/>
+      <c r="AE48" s="7"/>
+      <c r="AF48" s="7"/>
+      <c r="AG48" s="7"/>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
+        <v>43535</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="1">
+        <v>2001</v>
+      </c>
+      <c r="D49" t="s">
+        <v>91</v>
+      </c>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="U49" s="1"/>
+      <c r="V49" s="1"/>
+      <c r="W49" s="1"/>
+      <c r="X49" s="1"/>
+      <c r="Y49" s="1"/>
+      <c r="Z49" s="1"/>
+      <c r="AA49" s="1"/>
+      <c r="AB49" s="1"/>
+      <c r="AC49" s="1"/>
+      <c r="AD49" s="1"/>
+      <c r="AE49" s="1"/>
+      <c r="AF49" s="1"/>
+      <c r="AG49" s="1"/>
+    </row>
+    <row r="50" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="8">
+        <v>43535</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="7">
+        <v>-2001</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="7"/>
+      <c r="U50" s="7"/>
+      <c r="V50" s="7"/>
+      <c r="W50" s="7"/>
+      <c r="X50" s="7"/>
+      <c r="Y50" s="7"/>
+      <c r="Z50" s="7"/>
+      <c r="AA50" s="7"/>
+      <c r="AB50" s="7"/>
+      <c r="AC50" s="7"/>
+      <c r="AD50" s="7"/>
+      <c r="AE50" s="7"/>
+      <c r="AF50" s="7"/>
+      <c r="AG50" s="7"/>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+      <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
+      <c r="W51" s="1"/>
+      <c r="X51" s="1"/>
+      <c r="Y51" s="1"/>
+      <c r="Z51" s="1"/>
+      <c r="AA51" s="1"/>
+      <c r="AB51" s="1"/>
+      <c r="AC51" s="1"/>
+      <c r="AD51" s="1"/>
+      <c r="AE51" s="1"/>
+      <c r="AF51" s="1"/>
+      <c r="AG51" s="1"/>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" s="1">
+        <v>10</v>
+      </c>
+      <c r="D52" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="1">
+        <v>10</v>
+      </c>
+      <c r="D53" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" s="1">
+        <v>10</v>
+      </c>
+      <c r="D54" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A56" s="5">
+        <v>43171</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="1">
+        <v>10</v>
+      </c>
+      <c r="D56" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A57" s="5">
+        <v>43171</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57" s="1">
+        <v>10</v>
+      </c>
+      <c r="D57" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A58" s="5">
+        <v>43171</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C58" s="1">
+        <v>10</v>
+      </c>
+      <c r="D58" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A60" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60" s="1">
+        <v>100</v>
+      </c>
+      <c r="D60" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A61" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C61" s="1">
+        <v>100</v>
+      </c>
+      <c r="D61" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A62" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C62" s="1">
+        <v>100</v>
+      </c>
+      <c r="D62" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A63" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C63" s="1">
+        <v>100</v>
+      </c>
+      <c r="D63" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A64" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C64" s="1">
+        <v>100</v>
+      </c>
+      <c r="D64" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C65" s="1">
+        <v>100</v>
+      </c>
+      <c r="D65" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="8">
+        <v>43780</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C66" s="7">
+        <v>-100</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67" s="1">
+        <v>100</v>
+      </c>
+      <c r="D67" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="8">
+        <v>43780</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C68" s="7">
+        <v>-100</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="H68" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C69" s="1">
+        <v>100</v>
+      </c>
+      <c r="D69" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C70" s="1">
+        <v>100</v>
+      </c>
+      <c r="D70" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C71" s="1">
+        <v>100</v>
+      </c>
+      <c r="D71" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C72" s="1">
+        <v>102</v>
+      </c>
+      <c r="D72" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C73" s="1">
+        <v>102</v>
+      </c>
+      <c r="D73" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C74" s="1">
+        <v>102</v>
+      </c>
+      <c r="D74" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C75" s="1">
+        <v>102</v>
+      </c>
+      <c r="D75" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C76" s="1">
+        <v>102</v>
+      </c>
+      <c r="D76" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C77" s="1">
+        <v>102</v>
+      </c>
+      <c r="D77" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C80" s="1">
+        <v>101</v>
+      </c>
+      <c r="D80" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C81" s="1">
+        <v>101</v>
+      </c>
+      <c r="D81" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C82" s="1">
+        <v>101</v>
+      </c>
+      <c r="D82" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C83" s="1">
+        <v>101</v>
+      </c>
+      <c r="D83" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C84" s="1">
+        <v>101</v>
+      </c>
+      <c r="D84" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C85" s="1">
+        <v>101</v>
+      </c>
+      <c r="D85" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C86" s="1">
+        <v>101</v>
+      </c>
+      <c r="D86" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C87" s="1">
+        <v>101</v>
+      </c>
+      <c r="D87" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="8">
+        <v>43780</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C88" s="7">
+        <v>-101</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H88" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C89" s="1">
+        <v>101</v>
+      </c>
+      <c r="D89" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C90" s="1">
+        <v>101</v>
+      </c>
+      <c r="D90" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C91" s="1">
+        <v>101</v>
+      </c>
+      <c r="D91" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C92" s="1">
+        <v>101</v>
+      </c>
+      <c r="D92" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C93" s="1">
+        <v>101</v>
+      </c>
+      <c r="D93" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C94" s="1">
+        <v>101</v>
+      </c>
+      <c r="D94" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C95" s="1">
+        <v>101</v>
+      </c>
+      <c r="D95" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C96" s="1">
+        <v>101</v>
+      </c>
+      <c r="D96" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C98" s="1">
+        <v>1060</v>
+      </c>
+      <c r="D98" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C99" s="1">
+        <v>1060</v>
+      </c>
+      <c r="D99" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C100" s="1">
+        <v>1060</v>
+      </c>
+      <c r="D100" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C101" s="1">
+        <v>1060</v>
+      </c>
+      <c r="D101" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C102" s="1">
+        <v>1060</v>
+      </c>
+      <c r="D102" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C103" s="1">
+        <v>1060</v>
+      </c>
+      <c r="D103" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C104" s="1">
+        <v>1060</v>
+      </c>
+      <c r="D104" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C105" s="1">
+        <v>1060</v>
+      </c>
+      <c r="D105" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C107" s="1">
+        <v>1040</v>
+      </c>
+      <c r="D107" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C108" s="1">
+        <v>1040</v>
+      </c>
+      <c r="D108" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C109" s="1">
+        <v>1040</v>
+      </c>
+      <c r="D109" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C110" s="1">
+        <v>1040</v>
+      </c>
+      <c r="D110" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C111" s="1">
+        <v>-1040</v>
+      </c>
+      <c r="D111" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C112" s="1">
+        <v>-1040</v>
+      </c>
+      <c r="D112" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C113" s="1">
+        <v>1040</v>
+      </c>
+      <c r="D113" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use experiment names, more semicolons, and some plotting fixes
</commit_message>
<xml_diff>
--- a/3D networks data.xlsx
+++ b/3D networks data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20352"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20353"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niv\Documents\MATLAB\Maya code GUI - Niv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CED256C-1D97-4AB8-AA15-1FBA0840B7CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F45236-632E-47EC-B64A-EF8BC58EFD7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19185" windowHeight="7035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="258">
   <si>
     <t>Date</t>
   </si>
@@ -676,6 +676,129 @@
   </si>
   <si>
     <t>W:\phkinnerets\storage\analysis\Niv\rambam10\40%\2019_12_03\30um\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_12_11\30um\mix2 sample3\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_12_11\30um\mix2 sample3\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_12_11\30um\mix2 sample3\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_12_11\30um\mix2 sample3\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_12_11\30um\mix2 sample3\Capture 9</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_12_11\30um\mix2 sample3\Capture 10</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_12_11\30um\mix3 sample3\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_12_11\30um\mix3 sample3\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_12_11\30um\mix3 sample3\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_12_11\30um\mix3 sample3\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\I-phase\2019_12_11\30um\mix3 sample3\Capture 9</t>
+  </si>
+  <si>
+    <t>17/12/2019</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_17\mix1 sample3\Capture 1</t>
+  </si>
+  <si>
+    <t>Rambam 10 + 0.5uM ActA</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_17\mix1 sample3\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_17\mix1 sample3\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_17\mix1 sample3\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_17\mix1 sample3\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_17\mix1 sample3\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_17\mix1 sample3\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_17\mix1 sample3\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_17\mix2 sample3\Capture 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_17\mix2 sample3\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_17\mix2 sample3\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_17\mix2 sample3\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_17\mix2 sample3\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_17\mix2 sample3\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_17\mix2 sample3\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_17\mix2 sample3\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_17\mix2 sample3\Capture 9</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_17\mix2 sample3\Capture 10</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_19\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_19\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_19\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_19\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_19\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_19\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_19\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_19\Capture 9</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\ActA\30um\2019_12_19\Capture 10</t>
+  </si>
+  <si>
+    <t>19/12/2019</t>
   </si>
 </sst>
 </file>
@@ -1025,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BF163"/>
+  <dimension ref="A1:BF201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="B161" sqref="B161"/>
+    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
+      <selection activeCell="D195" sqref="D195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2522,7 +2645,7 @@
         <v>116</v>
       </c>
       <c r="C95" s="1">
-        <v>102</v>
+        <v>-102</v>
       </c>
       <c r="D95" s="6" t="s">
         <v>148</v>
@@ -2553,7 +2676,7 @@
         <v>116</v>
       </c>
       <c r="C97" s="1">
-        <v>102</v>
+        <v>-102</v>
       </c>
       <c r="D97" s="6" t="s">
         <v>150</v>
@@ -2884,147 +3007,158 @@
         <v>211</v>
       </c>
     </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="5">
+        <v>43781</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C121" s="1">
+        <v>104</v>
+      </c>
+      <c r="D121" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="5">
+        <v>43781</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C122" s="1">
+        <v>104</v>
+      </c>
+      <c r="D122" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="5">
+        <v>43781</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C123" s="1">
+        <v>-104</v>
+      </c>
+      <c r="D123" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="5">
+        <v>43781</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C124" s="1">
+        <v>104</v>
+      </c>
+      <c r="D124" t="s">
+        <v>220</v>
+      </c>
+    </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="5">
-        <v>43780</v>
+        <v>43781</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C125" s="1">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D125" t="s">
-        <v>118</v>
+        <v>221</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
-        <v>43780</v>
+        <v>43781</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C126" s="1">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D126" t="s">
-        <v>119</v>
+        <v>222</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="5">
-        <v>43780</v>
+        <v>43781</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C127" s="1">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D127" t="s">
-        <v>120</v>
+        <v>223</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="5">
-        <v>43780</v>
+        <v>43781</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C128" s="1">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D128" t="s">
-        <v>129</v>
+        <v>224</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="5">
-        <v>43780</v>
+        <v>43781</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C129" s="1">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D129" t="s">
-        <v>121</v>
+        <v>225</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="5">
-        <v>43780</v>
+        <v>43781</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C130" s="1">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D130" t="s">
-        <v>128</v>
+        <v>226</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="5">
-        <v>43780</v>
+        <v>43781</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C131" s="1">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D131" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A132" s="5">
-        <v>43780</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C132" s="1">
-        <v>101</v>
-      </c>
-      <c r="D132" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="8">
-        <v>43780</v>
-      </c>
-      <c r="B133" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C133" s="7">
-        <v>-101</v>
-      </c>
-      <c r="D133" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="H133" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A134" s="5">
-        <v>43780</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C134" s="1">
-        <v>101</v>
-      </c>
-      <c r="D134" t="s">
-        <v>131</v>
+        <v>227</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -3038,7 +3172,7 @@
         <v>101</v>
       </c>
       <c r="D135" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -3052,7 +3186,7 @@
         <v>101</v>
       </c>
       <c r="D136" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -3066,7 +3200,7 @@
         <v>101</v>
       </c>
       <c r="D137" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -3080,7 +3214,7 @@
         <v>101</v>
       </c>
       <c r="D138" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -3094,7 +3228,7 @@
         <v>101</v>
       </c>
       <c r="D139" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -3108,7 +3242,7 @@
         <v>101</v>
       </c>
       <c r="D140" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -3122,133 +3256,150 @@
         <v>101</v>
       </c>
       <c r="D141" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A142" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C142" s="1">
+        <v>101</v>
+      </c>
+      <c r="D142" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="8">
+        <v>43780</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C143" s="7">
+        <v>-101</v>
+      </c>
+      <c r="D143" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H143" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A144" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C144" s="1">
+        <v>101</v>
+      </c>
+      <c r="D144" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C145" s="1">
+        <v>101</v>
+      </c>
+      <c r="D145" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C146" s="1">
+        <v>101</v>
+      </c>
+      <c r="D146" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C147" s="1">
+        <v>101</v>
+      </c>
+      <c r="D147" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C148" s="1">
+        <v>101</v>
+      </c>
+      <c r="D148" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C149" s="1">
+        <v>101</v>
+      </c>
+      <c r="D149" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C150" s="1">
+        <v>101</v>
+      </c>
+      <c r="D150" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="5">
+        <v>43780</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C151" s="1">
+        <v>101</v>
+      </c>
+      <c r="D151" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A143" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C143" s="1">
-        <v>1060</v>
-      </c>
-      <c r="D143" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A144" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C144" s="1">
-        <v>1060</v>
-      </c>
-      <c r="D144" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B145" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C145" s="1">
-        <v>1060</v>
-      </c>
-      <c r="D145" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C146" s="1">
-        <v>1060</v>
-      </c>
-      <c r="D146" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C147" s="1">
-        <v>1060</v>
-      </c>
-      <c r="D147" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C148" s="1">
-        <v>1060</v>
-      </c>
-      <c r="D148" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C149" s="1">
-        <v>1060</v>
-      </c>
-      <c r="D149" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C150" s="1">
-        <v>1060</v>
-      </c>
-      <c r="D150" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C152" s="1">
-        <v>1040</v>
-      </c>
-      <c r="D152" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -3256,13 +3407,13 @@
         <v>141</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="C153" s="1">
-        <v>1040</v>
+        <v>1060</v>
       </c>
       <c r="D153" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -3270,13 +3421,13 @@
         <v>141</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="C154" s="1">
-        <v>1040</v>
+        <v>1060</v>
       </c>
       <c r="D154" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -3284,41 +3435,41 @@
         <v>141</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="C155" s="1">
-        <v>1040</v>
+        <v>1060</v>
       </c>
       <c r="D155" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B156" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="C156" s="7">
-        <v>-1040</v>
-      </c>
-      <c r="D156" s="6" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="8" t="s">
+      <c r="B156" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C156" s="1">
+        <v>1060</v>
+      </c>
+      <c r="D156" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B157" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="C157" s="7">
-        <v>-1040</v>
-      </c>
-      <c r="D157" s="6" t="s">
-        <v>168</v>
+      <c r="B157" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C157" s="1">
+        <v>1060</v>
+      </c>
+      <c r="D157" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -3326,83 +3477,587 @@
         <v>141</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="C158" s="1">
-        <v>1040</v>
+        <v>1060</v>
       </c>
       <c r="D158" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="5">
-        <v>43536</v>
+      <c r="A159" s="5" t="s">
+        <v>141</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="C159" s="1">
-        <v>1041</v>
+        <v>1060</v>
       </c>
       <c r="D159" t="s">
-        <v>212</v>
+        <v>161</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="5">
-        <v>43536</v>
+      <c r="A160" s="5" t="s">
+        <v>141</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="C160" s="1">
-        <v>1041</v>
+        <v>1060</v>
       </c>
       <c r="D160" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="5">
-        <v>43536</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C161" s="1">
-        <v>1041</v>
-      </c>
-      <c r="D161" t="s">
-        <v>214</v>
+        <v>162</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="5">
-        <v>43536</v>
+      <c r="A162" s="5" t="s">
+        <v>141</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>170</v>
       </c>
       <c r="C162" s="1">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D162" t="s">
-        <v>215</v>
+        <v>163</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="5">
-        <v>43536</v>
+      <c r="A163" s="5" t="s">
+        <v>141</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>170</v>
       </c>
       <c r="C163" s="1">
+        <v>1040</v>
+      </c>
+      <c r="D163" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C164" s="1">
+        <v>1040</v>
+      </c>
+      <c r="D164" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C165" s="1">
+        <v>1040</v>
+      </c>
+      <c r="D165" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B166" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C166" s="7">
+        <v>-1040</v>
+      </c>
+      <c r="D166" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B167" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C167" s="7">
+        <v>-1040</v>
+      </c>
+      <c r="D167" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C168" s="1">
+        <v>1043</v>
+      </c>
+      <c r="D168" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="5">
+        <v>43536</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C169" s="1">
         <v>1041</v>
       </c>
-      <c r="D163" t="s">
+      <c r="D169" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="5">
+        <v>43536</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C170" s="1">
+        <v>1041</v>
+      </c>
+      <c r="D170" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="5">
+        <v>43536</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C171" s="1">
+        <v>1041</v>
+      </c>
+      <c r="D171" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="5">
+        <v>43536</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C172" s="1">
+        <v>1041</v>
+      </c>
+      <c r="D172" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="5">
+        <v>43536</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C173" s="1">
+        <v>1041</v>
+      </c>
+      <c r="D173" t="s">
         <v>216</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C175" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D175" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C176" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D176" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C177" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D177" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C178" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D178" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C179" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D179" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C180" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D180" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C181" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D181" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C182" s="1">
+        <v>-1030</v>
+      </c>
+      <c r="D182" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C183" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D183" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C184" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D184" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C185" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D185" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C186" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D186" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C187" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D187" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C188" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D188" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C189" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D189" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C190" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D190" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C191" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D191" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C192" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D192" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C193" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D193" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C194" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D194" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C195" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D195" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C196" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D196" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C197" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D197" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C198" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D198" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C199" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D199" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C200" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D200" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C201" s="1">
+        <v>1030</v>
+      </c>
+      <c r="D201" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature: add brightness slider to droplet measure image
</commit_message>
<xml_diff>
--- a/3D networks data.xlsx
+++ b/3D networks data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20353"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niv\Documents\MATLAB\Maya code GUI - Niv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nivieru\Documents\MATLAB\Maya code GUI - Niv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F45236-632E-47EC-B64A-EF8BC58EFD7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20553803-4206-4752-8F5B-A6430A47B887}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19185" windowHeight="7035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19183" windowHeight="7037" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="329">
   <si>
     <t>Date</t>
   </si>
@@ -799,6 +799,219 @@
   </si>
   <si>
     <t>19/12/2019</t>
+  </si>
+  <si>
+    <t>Rambam 10 95%</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_07_14\sample1 63x\Capture 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_07_14\sample1 63x\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_07_14\sample1 63x\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_07_14\sample1 63x\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_07_14\sample1 63x\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_07_14\sample1 63x\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_07_14\sample1 63x\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_07_14\sample1 63x\Capture 13</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_08\Capture 1</t>
+  </si>
+  <si>
+    <t>Rambam 10 95% no EGTA</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_08\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_08\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_08\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_08\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_08\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_08\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_08\Capture 8</t>
+  </si>
+  <si>
+    <t>Rambam 17 95% 12mM Mg</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\Rambam17\95% with 12mM Mg\2020_11_11 mix1\sample1 63x\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\Rambam17\95% with 12mM Mg\2020_11_11 mix1\sample1 63x\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\Rambam17\95% with 12mM Mg\2020_11_11 mix1\sample1 63x\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\Rambam17\95% with 12mM Mg\2020_11_11 mix1\sample1 63x\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\Rambam17\95% with 12mM Mg\2020_11_11 mix1\sample2 63x\Capture 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\Rambam17\95% with 12mM Mg\2020_11_11 mix1\sample2 63x\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\Rambam17\95% with 12mM Mg\2020_11_11 mix1\sample2 63x\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\Rambam17\95% with 12mM Mg\2020_11_11 mix1\sample2 63x\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\Rambam17\95% with 12mM Mg\2020_11_11 mix1\sample2 63x\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\Rambam17\95% with DDW\2020_11_11 mix2\63x\Capture 5</t>
+  </si>
+  <si>
+    <t>Rambam 17 95% with DDW</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\Rambam17\95% with DDW\2020_11_11 mix2\63x\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\Rambam17\95% with DDW\2020_11_11 mix2\63x\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\Rambam17\95% with DDW\2020_11_11 mix2\63x\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\Rambam17\95% with 2% DMSO\2020_11_11 mix3\63x\Capture 6</t>
+  </si>
+  <si>
+    <t>Rambam 17 95% with 2% DMSO</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\Rambam17\95% with 2% DMSO\2020_11_11 mix3\63x\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\Rambam17\95% with 2% DMSO\2020_11_11 mix3\63x\Capture 8</t>
+  </si>
+  <si>
+    <t>Rambam 17 95% with DDW at 18 degrees</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\Rambam17\95% with DDW at 18 degrees\2020_11_11 mix4\63x\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\Rambam17\95% with DDW at 18 degrees\2020_11_11 mix4\63x\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\Rambam17\95% with DDW at 18 degrees\2020_11_11 mix4\63x\Capture 6</t>
+  </si>
+  <si>
+    <t>11-17-2020</t>
+  </si>
+  <si>
+    <t>Rambam 10 95% 13mM Mg no EGTA</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix1 95% rambam10 with 13mM Mg\63x\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix1 95% rambam10 with 13mM Mg\63x\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix1 95% rambam10 with 13mM Mg\63x\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix1 95% rambam10 with 13mM Mg\63x\Capture 12</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix3 95% rambam10 with 7mM Mg\63x\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix3 95% rambam10 with 7mM Mg\63x\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix3 95% rambam10 with 7mM Mg\63x\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix3 95% rambam10 with 7mM Mg\63x\Capture 8</t>
+  </si>
+  <si>
+    <t>Rambam 10 95% 7mM Mg no EGTA</t>
+  </si>
+  <si>
+    <t>Rambam 10 95% 26mM Mg no EGTA</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix2 95% rambam10 with 26mM Mg\63x\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix2 95% rambam10 with 26mM Mg\63x\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix2 95% rambam10 with 26mM Mg\63x\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix1 95% rambam10 with 300nM calyculin sample1\63x\Capture 5</t>
+  </si>
+  <si>
+    <t>Rambam 10 95% 300nM calyculin no EGTA</t>
+  </si>
+  <si>
+    <t>11-19-2020</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix1 95% rambam10 with 300nM calyculin sample1\63x\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix1 95% rambam10 with 300nM calyculin sample2\63x\Capture 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix1 95% rambam10 with 300nM calyculin sample2\63x\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix1 95% rambam10 with 300nM calyculin sample2\63x\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix1 95% rambam10 with 300nM calyculin sample2\63x\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix1 95% rambam10 with 300nM calyculin sample2\63x\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix1 95% rambam10 with 300nM calyculin sample2\63x\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix1 95% rambam10 with 300nM calyculin sample2\63x\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix1 95% rambam10 with 300nM calyculin sample2\63x\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix1 95% rambam10 with 300nM calyculin sample2\63x\Capture 9</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix1 95% rambam10 with 300nM calyculin sample2\63x\Capture 10</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix1 95% rambam10 with 300nM calyculin sample2\63x\Capture 11</t>
   </si>
 </sst>
 </file>
@@ -1148,21 +1361,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BF201"/>
+  <dimension ref="A1:BF283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="D195" sqref="D195"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="B219" sqref="B219"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="41.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="61.5703125" customWidth="1"/>
+    <col min="1" max="1" width="26.84375" customWidth="1"/>
+    <col min="2" max="2" width="41.15234375" customWidth="1"/>
+    <col min="3" max="3" width="24.3046875" customWidth="1"/>
+    <col min="4" max="4" width="61.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" s="4" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" s="4" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1338,7 +1551,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.4">
       <c r="A2" s="5">
         <v>43376</v>
       </c>
@@ -1370,7 +1583,7 @@
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.4">
       <c r="A3" s="5">
         <v>43376</v>
       </c>
@@ -1384,7 +1597,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.4">
       <c r="A4" s="5">
         <v>43376</v>
       </c>
@@ -1398,7 +1611,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.4">
       <c r="A5" s="5">
         <v>43376</v>
       </c>
@@ -1412,7 +1625,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.4">
       <c r="A6" s="5">
         <v>43376</v>
       </c>
@@ -1426,7 +1639,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.4">
       <c r="A8" s="5">
         <v>43503</v>
       </c>
@@ -1440,7 +1653,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.4">
       <c r="A9" s="5">
         <v>43503</v>
       </c>
@@ -1454,7 +1667,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.4">
       <c r="A10" s="5">
         <v>43503</v>
       </c>
@@ -1468,7 +1681,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.4">
       <c r="A11" s="5">
         <v>43503</v>
       </c>
@@ -1482,7 +1695,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.4">
       <c r="A12" s="5">
         <v>43503</v>
       </c>
@@ -1496,7 +1709,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.4">
       <c r="A13" s="5">
         <v>43503</v>
       </c>
@@ -1510,7 +1723,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.4">
       <c r="A14" s="5">
         <v>43503</v>
       </c>
@@ -1524,7 +1737,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.4">
       <c r="A15" s="5">
         <v>43503</v>
       </c>
@@ -1538,7 +1751,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>20170808</v>
       </c>
@@ -1552,7 +1765,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>20170808</v>
       </c>
@@ -1566,7 +1779,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>20170808</v>
       </c>
@@ -1580,7 +1793,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>20170808</v>
       </c>
@@ -1594,7 +1807,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>20170808</v>
       </c>
@@ -1608,11 +1821,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>20170815</v>
       </c>
@@ -1626,7 +1839,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24">
         <v>20170815</v>
       </c>
@@ -1640,7 +1853,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25">
         <v>20170815</v>
       </c>
@@ -1654,7 +1867,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26">
         <v>20170815</v>
       </c>
@@ -1668,7 +1881,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27">
         <v>20170815</v>
       </c>
@@ -1682,7 +1895,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28">
         <v>20170815</v>
       </c>
@@ -1696,7 +1909,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A29">
         <v>20170815</v>
       </c>
@@ -1710,7 +1923,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A30">
         <v>20170815</v>
       </c>
@@ -1724,7 +1937,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31">
         <v>20171221</v>
       </c>
@@ -1738,7 +1951,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A32">
         <v>20171221</v>
       </c>
@@ -1752,7 +1965,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A33">
         <v>20171221</v>
       </c>
@@ -1766,7 +1979,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A34">
         <v>20171221</v>
       </c>
@@ -1780,7 +1993,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A35">
         <v>20171221</v>
       </c>
@@ -1794,7 +2007,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A36">
         <v>20171221</v>
       </c>
@@ -1808,11 +2021,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.4">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A38" s="5">
         <v>43535</v>
       </c>
@@ -1826,7 +2039,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A39" s="5">
         <v>43535</v>
       </c>
@@ -1840,7 +2053,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A40" s="5">
         <v>43535</v>
       </c>
@@ -1854,7 +2067,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A41" s="5">
         <v>43535</v>
       </c>
@@ -1868,7 +2081,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A42" s="5">
         <v>43535</v>
       </c>
@@ -1882,7 +2095,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A43" s="5">
         <v>43535</v>
       </c>
@@ -1896,7 +2109,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A44" s="8">
         <v>43535</v>
       </c>
@@ -1913,7 +2126,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A45" s="8">
         <v>43535</v>
       </c>
@@ -1930,7 +2143,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A46" s="8">
         <v>43535</v>
       </c>
@@ -1965,7 +2178,7 @@
       <c r="AF46" s="7"/>
       <c r="AG46" s="7"/>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A47" s="5">
         <v>43535</v>
       </c>
@@ -1997,7 +2210,7 @@
       <c r="AF47" s="1"/>
       <c r="AG47" s="1"/>
     </row>
-    <row r="48" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A48" s="8">
         <v>43535</v>
       </c>
@@ -2032,7 +2245,7 @@
       <c r="AF48" s="7"/>
       <c r="AG48" s="7"/>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A49" s="5">
         <v>43535</v>
       </c>
@@ -2064,7 +2277,7 @@
       <c r="AF49" s="1"/>
       <c r="AG49" s="1"/>
     </row>
-    <row r="50" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A50" s="8">
         <v>43535</v>
       </c>
@@ -2099,7 +2312,7 @@
       <c r="AF50" s="7"/>
       <c r="AG50" s="7"/>
     </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.4">
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
@@ -2119,7 +2332,7 @@
       <c r="AF51" s="1"/>
       <c r="AG51" s="1"/>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A52" s="5" t="s">
         <v>113</v>
       </c>
@@ -2133,7 +2346,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A53" s="5" t="s">
         <v>113</v>
       </c>
@@ -2147,7 +2360,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A54" s="5" t="s">
         <v>113</v>
       </c>
@@ -2161,7 +2374,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A56" s="5">
         <v>43171</v>
       </c>
@@ -2175,7 +2388,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A57" s="5">
         <v>43171</v>
       </c>
@@ -2189,7 +2402,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A58" s="5">
         <v>43171</v>
       </c>
@@ -2203,7 +2416,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A59" s="5" t="s">
         <v>179</v>
       </c>
@@ -2217,7 +2430,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A60" s="5" t="s">
         <v>179</v>
       </c>
@@ -2231,7 +2444,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A61" s="5" t="s">
         <v>179</v>
       </c>
@@ -2245,7 +2458,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A62" s="5" t="s">
         <v>179</v>
       </c>
@@ -2259,7 +2472,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">
         <v>179</v>
       </c>
@@ -2273,7 +2486,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
         <v>179</v>
       </c>
@@ -2287,7 +2500,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A65" s="5" t="s">
         <v>179</v>
       </c>
@@ -2301,7 +2514,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A67" s="5">
         <v>43567</v>
       </c>
@@ -2315,7 +2528,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A68" s="5">
         <v>43567</v>
       </c>
@@ -2329,7 +2542,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A69" s="5">
         <v>43567</v>
       </c>
@@ -2343,7 +2556,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A70" s="5">
         <v>43567</v>
       </c>
@@ -2357,7 +2570,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A71" s="5">
         <v>43567</v>
       </c>
@@ -2371,7 +2584,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A72" s="5">
         <v>43567</v>
       </c>
@@ -2385,7 +2598,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A73" s="5">
         <v>43567</v>
       </c>
@@ -2399,7 +2612,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A74" s="5">
         <v>43567</v>
       </c>
@@ -2413,7 +2626,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A75" s="5">
         <v>43567</v>
       </c>
@@ -2427,7 +2640,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A76" s="5">
         <v>43567</v>
       </c>
@@ -2441,7 +2654,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A78" s="5">
         <v>43567</v>
       </c>
@@ -2455,7 +2668,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A79" s="5">
         <v>43567</v>
       </c>
@@ -2469,7 +2682,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A80" s="5">
         <v>43567</v>
       </c>
@@ -2483,7 +2696,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A81" s="5">
         <v>43567</v>
       </c>
@@ -2497,7 +2710,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A82" s="5">
         <v>43567</v>
       </c>
@@ -2511,7 +2724,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A83" s="5">
         <v>43567</v>
       </c>
@@ -2525,7 +2738,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A84" s="5">
         <v>43567</v>
       </c>
@@ -2539,7 +2752,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A85" s="5">
         <v>43567</v>
       </c>
@@ -2553,7 +2766,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A89" s="5">
         <v>43780</v>
       </c>
@@ -2567,7 +2780,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A90" s="5">
         <v>43780</v>
       </c>
@@ -2581,7 +2794,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A91" s="5">
         <v>43780</v>
       </c>
@@ -2595,7 +2808,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A92" s="5">
         <v>43780</v>
       </c>
@@ -2609,7 +2822,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A93" s="5">
         <v>43780</v>
       </c>
@@ -2623,7 +2836,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A94" s="5">
         <v>43780</v>
       </c>
@@ -2637,7 +2850,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="95" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A95" s="8">
         <v>43780</v>
       </c>
@@ -2654,7 +2867,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A96" s="5">
         <v>43780</v>
       </c>
@@ -2668,7 +2881,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="97" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A97" s="8">
         <v>43780</v>
       </c>
@@ -2685,7 +2898,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A98" s="5">
         <v>43780</v>
       </c>
@@ -2699,7 +2912,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A99" s="5">
         <v>43780</v>
       </c>
@@ -2713,7 +2926,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A100" s="5">
         <v>43780</v>
       </c>
@@ -2727,7 +2940,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A101" s="5" t="s">
         <v>141</v>
       </c>
@@ -2741,7 +2954,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A102" s="5" t="s">
         <v>141</v>
       </c>
@@ -2755,7 +2968,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A103" s="5" t="s">
         <v>141</v>
       </c>
@@ -2769,7 +2982,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A104" s="5" t="s">
         <v>141</v>
       </c>
@@ -2783,7 +2996,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A105" s="5" t="s">
         <v>141</v>
       </c>
@@ -2797,7 +3010,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A106" s="5" t="s">
         <v>141</v>
       </c>
@@ -2811,7 +3024,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A107" s="5" t="s">
         <v>203</v>
       </c>
@@ -2825,7 +3038,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A108" s="5" t="s">
         <v>203</v>
       </c>
@@ -2839,7 +3052,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A109" s="5" t="s">
         <v>203</v>
       </c>
@@ -2853,7 +3066,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A110" s="5" t="s">
         <v>203</v>
       </c>
@@ -2867,7 +3080,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A111" s="5" t="s">
         <v>203</v>
       </c>
@@ -2881,7 +3094,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A112" s="5" t="s">
         <v>203</v>
       </c>
@@ -2895,7 +3108,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A113" s="5" t="s">
         <v>203</v>
       </c>
@@ -2909,7 +3122,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A114" s="5" t="s">
         <v>203</v>
       </c>
@@ -2923,7 +3136,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A115" s="5" t="s">
         <v>203</v>
       </c>
@@ -2937,7 +3150,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A116" s="5" t="s">
         <v>203</v>
       </c>
@@ -2951,7 +3164,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A117" s="5" t="s">
         <v>203</v>
       </c>
@@ -2965,7 +3178,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A118" s="5" t="s">
         <v>203</v>
       </c>
@@ -2979,7 +3192,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A119" s="5" t="s">
         <v>203</v>
       </c>
@@ -2993,7 +3206,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A120" s="5" t="s">
         <v>203</v>
       </c>
@@ -3007,7 +3220,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A121" s="5">
         <v>43781</v>
       </c>
@@ -3021,7 +3234,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A122" s="5">
         <v>43781</v>
       </c>
@@ -3035,7 +3248,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A123" s="5">
         <v>43781</v>
       </c>
@@ -3049,7 +3262,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A124" s="5">
         <v>43781</v>
       </c>
@@ -3063,7 +3276,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A125" s="5">
         <v>43781</v>
       </c>
@@ -3077,7 +3290,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A126" s="5">
         <v>43781</v>
       </c>
@@ -3091,7 +3304,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A127" s="5">
         <v>43781</v>
       </c>
@@ -3105,7 +3318,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A128" s="5">
         <v>43781</v>
       </c>
@@ -3119,7 +3332,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A129" s="5">
         <v>43781</v>
       </c>
@@ -3133,7 +3346,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A130" s="5">
         <v>43781</v>
       </c>
@@ -3147,7 +3360,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A131" s="5">
         <v>43781</v>
       </c>
@@ -3161,7 +3374,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A135" s="5">
         <v>43780</v>
       </c>
@@ -3175,7 +3388,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A136" s="5">
         <v>43780</v>
       </c>
@@ -3189,7 +3402,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A137" s="5">
         <v>43780</v>
       </c>
@@ -3203,7 +3416,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A138" s="5">
         <v>43780</v>
       </c>
@@ -3217,7 +3430,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A139" s="5">
         <v>43780</v>
       </c>
@@ -3231,7 +3444,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A140" s="5">
         <v>43780</v>
       </c>
@@ -3245,7 +3458,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A141" s="5">
         <v>43780</v>
       </c>
@@ -3259,7 +3472,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A142" s="5">
         <v>43780</v>
       </c>
@@ -3273,7 +3486,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="143" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A143" s="8">
         <v>43780</v>
       </c>
@@ -3290,7 +3503,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A144" s="5">
         <v>43780</v>
       </c>
@@ -3304,7 +3517,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A145" s="5">
         <v>43780</v>
       </c>
@@ -3318,7 +3531,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A146" s="5">
         <v>43780</v>
       </c>
@@ -3332,7 +3545,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A147" s="5">
         <v>43780</v>
       </c>
@@ -3346,7 +3559,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A148" s="5">
         <v>43780</v>
       </c>
@@ -3360,7 +3573,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A149" s="5">
         <v>43780</v>
       </c>
@@ -3374,7 +3587,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A150" s="5">
         <v>43780</v>
       </c>
@@ -3388,7 +3601,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A151" s="5">
         <v>43780</v>
       </c>
@@ -3402,7 +3615,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A153" s="5" t="s">
         <v>141</v>
       </c>
@@ -3416,7 +3629,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A154" s="5" t="s">
         <v>141</v>
       </c>
@@ -3430,7 +3643,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A155" s="5" t="s">
         <v>141</v>
       </c>
@@ -3444,7 +3657,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A156" s="5" t="s">
         <v>141</v>
       </c>
@@ -3458,7 +3671,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A157" s="5" t="s">
         <v>141</v>
       </c>
@@ -3472,7 +3685,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A158" s="5" t="s">
         <v>141</v>
       </c>
@@ -3486,7 +3699,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A159" s="5" t="s">
         <v>141</v>
       </c>
@@ -3500,7 +3713,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A160" s="5" t="s">
         <v>141</v>
       </c>
@@ -3514,7 +3727,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A162" s="5" t="s">
         <v>141</v>
       </c>
@@ -3528,7 +3741,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A163" s="5" t="s">
         <v>141</v>
       </c>
@@ -3542,7 +3755,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A164" s="5" t="s">
         <v>141</v>
       </c>
@@ -3556,7 +3769,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A165" s="5" t="s">
         <v>141</v>
       </c>
@@ -3570,7 +3783,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="166" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A166" s="8" t="s">
         <v>141</v>
       </c>
@@ -3584,7 +3797,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="167" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A167" s="8" t="s">
         <v>141</v>
       </c>
@@ -3598,7 +3811,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A168" s="5" t="s">
         <v>141</v>
       </c>
@@ -3612,7 +3825,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A169" s="5">
         <v>43536</v>
       </c>
@@ -3626,7 +3839,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A170" s="5">
         <v>43536</v>
       </c>
@@ -3640,7 +3853,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A171" s="5">
         <v>43536</v>
       </c>
@@ -3654,7 +3867,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A172" s="5">
         <v>43536</v>
       </c>
@@ -3668,7 +3881,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A173" s="5">
         <v>43536</v>
       </c>
@@ -3682,7 +3895,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A175" s="5" t="s">
         <v>228</v>
       </c>
@@ -3696,7 +3909,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A176" s="5" t="s">
         <v>228</v>
       </c>
@@ -3710,7 +3923,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A177" s="5" t="s">
         <v>228</v>
       </c>
@@ -3724,7 +3937,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A178" s="5" t="s">
         <v>228</v>
       </c>
@@ -3738,7 +3951,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A179" s="5" t="s">
         <v>228</v>
       </c>
@@ -3752,7 +3965,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A180" s="5" t="s">
         <v>228</v>
       </c>
@@ -3766,7 +3979,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A181" s="5" t="s">
         <v>228</v>
       </c>
@@ -3780,7 +3993,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A182" s="5" t="s">
         <v>228</v>
       </c>
@@ -3794,7 +4007,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A183" s="5" t="s">
         <v>228</v>
       </c>
@@ -3808,7 +4021,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A184" s="5" t="s">
         <v>228</v>
       </c>
@@ -3822,7 +4035,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A185" s="5" t="s">
         <v>228</v>
       </c>
@@ -3836,7 +4049,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A186" s="5" t="s">
         <v>228</v>
       </c>
@@ -3850,7 +4063,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A187" s="5" t="s">
         <v>228</v>
       </c>
@@ -3864,7 +4077,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A188" s="5" t="s">
         <v>228</v>
       </c>
@@ -3878,7 +4091,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A189" s="5" t="s">
         <v>228</v>
       </c>
@@ -3892,7 +4105,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A190" s="5" t="s">
         <v>228</v>
       </c>
@@ -3906,7 +4119,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A191" s="5" t="s">
         <v>228</v>
       </c>
@@ -3920,7 +4133,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A192" s="5" t="s">
         <v>228</v>
       </c>
@@ -3934,7 +4147,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A193" s="5" t="s">
         <v>257</v>
       </c>
@@ -3948,7 +4161,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A194" s="5" t="s">
         <v>257</v>
       </c>
@@ -3962,7 +4175,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A195" s="5" t="s">
         <v>257</v>
       </c>
@@ -3976,7 +4189,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A196" s="5" t="s">
         <v>257</v>
       </c>
@@ -3990,7 +4203,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A197" s="5" t="s">
         <v>257</v>
       </c>
@@ -4004,7 +4217,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A198" s="5" t="s">
         <v>257</v>
       </c>
@@ -4018,7 +4231,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A199" s="5" t="s">
         <v>257</v>
       </c>
@@ -4032,7 +4245,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A200" s="5" t="s">
         <v>257</v>
       </c>
@@ -4046,7 +4259,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A201" s="5" t="s">
         <v>257</v>
       </c>
@@ -4058,6 +4271,902 @@
       </c>
       <c r="D201" t="s">
         <v>256</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A203" s="5">
+        <v>44026</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C203" s="1">
+        <v>1095</v>
+      </c>
+      <c r="D203" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A204" s="5">
+        <v>44026</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C204" s="1">
+        <v>1095</v>
+      </c>
+      <c r="D204" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A205" s="5">
+        <v>44026</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C205" s="1">
+        <v>1095</v>
+      </c>
+      <c r="D205" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A206" s="5">
+        <v>44026</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C206" s="1">
+        <v>1095</v>
+      </c>
+      <c r="D206" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A207" s="5">
+        <v>44026</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C207" s="1">
+        <v>1095</v>
+      </c>
+      <c r="D207" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A208" s="5">
+        <v>44026</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C208" s="1">
+        <v>1095</v>
+      </c>
+      <c r="D208" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A209" s="5">
+        <v>44026</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C209" s="1">
+        <v>1095</v>
+      </c>
+      <c r="D209" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A210" s="5">
+        <v>44026</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C210" s="1">
+        <v>1095</v>
+      </c>
+      <c r="D210" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A212" s="5">
+        <v>44054</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C212" s="1">
+        <v>11095</v>
+      </c>
+      <c r="D212" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A213" s="5">
+        <v>44054</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C213" s="1">
+        <v>11095</v>
+      </c>
+      <c r="D213" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A214" s="5">
+        <v>44054</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C214" s="1">
+        <v>11095</v>
+      </c>
+      <c r="D214" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A215" s="5">
+        <v>44054</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C215" s="1">
+        <v>11095</v>
+      </c>
+      <c r="D215" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A216" s="5">
+        <v>44054</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C216" s="1">
+        <v>11095</v>
+      </c>
+      <c r="D216" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A217" s="5">
+        <v>44054</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C217" s="1">
+        <v>11095</v>
+      </c>
+      <c r="D217" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A218" s="5">
+        <v>44054</v>
+      </c>
+      <c r="B218" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C218" s="1">
+        <v>11095</v>
+      </c>
+      <c r="D218" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A219" s="5">
+        <v>44054</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C219" s="1">
+        <v>11095</v>
+      </c>
+      <c r="D219" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A221" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C221" s="1">
+        <v>131095</v>
+      </c>
+      <c r="D221" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A222" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C222" s="1">
+        <v>131095</v>
+      </c>
+      <c r="D222" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A223" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C223" s="1">
+        <v>131095</v>
+      </c>
+      <c r="D223" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A224" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C224" s="1">
+        <v>131095</v>
+      </c>
+      <c r="D224" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A226" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C226" s="1">
+        <v>71095</v>
+      </c>
+      <c r="D226" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A227" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C227" s="1">
+        <v>71095</v>
+      </c>
+      <c r="D227" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A228" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B228" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C228" s="1">
+        <v>71095</v>
+      </c>
+      <c r="D228" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A229" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C229" s="1">
+        <v>71095</v>
+      </c>
+      <c r="D229" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A231" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C231" s="1">
+        <v>261095</v>
+      </c>
+      <c r="D231" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A232" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B232" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C232" s="1">
+        <v>261095</v>
+      </c>
+      <c r="D232" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A233" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C233" s="1">
+        <v>261095</v>
+      </c>
+      <c r="D233" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A234" s="5"/>
+      <c r="B234" s="1"/>
+      <c r="C234" s="1"/>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A235" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C235" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D235" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A236" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C236" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D236" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A237" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C237" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D237" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A238" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C238" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D238" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A239" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C239" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D239" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A240" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C240" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D240" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A241" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C241" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D241" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A242" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B242" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C242" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D242" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A243" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C243" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D243" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A244" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C244" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D244" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A245" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C245" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D245" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A246" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B246" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C246" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D246" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A247" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C247" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D247" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A248" s="5"/>
+      <c r="B248" s="1"/>
+      <c r="C248" s="1"/>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A249" s="5"/>
+      <c r="B249" s="1"/>
+      <c r="C249" s="1"/>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A250" s="5"/>
+      <c r="B250" s="1"/>
+      <c r="C250" s="1"/>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A251" s="5"/>
+      <c r="B251" s="1"/>
+      <c r="C251" s="1"/>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A252" s="5"/>
+      <c r="B252" s="1"/>
+      <c r="C252" s="1"/>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A253" s="5"/>
+      <c r="B253" s="1"/>
+      <c r="C253" s="1"/>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A254" s="5"/>
+      <c r="B254" s="1"/>
+      <c r="C254" s="1"/>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A255" s="5"/>
+      <c r="B255" s="1"/>
+      <c r="C255" s="1"/>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A256" s="5"/>
+      <c r="B256" s="1"/>
+      <c r="C256" s="1"/>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A257" s="5"/>
+      <c r="B257" s="1"/>
+      <c r="C257" s="1"/>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A258" s="5"/>
+      <c r="B258" s="1"/>
+      <c r="C258" s="1"/>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A259" s="5"/>
+      <c r="B259" s="1"/>
+      <c r="C259" s="1"/>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A260" s="5"/>
+      <c r="B260" s="1"/>
+      <c r="C260" s="1"/>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A262" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C262" s="1">
+        <v>121795</v>
+      </c>
+      <c r="D262" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A263" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C263" s="1">
+        <v>121795</v>
+      </c>
+      <c r="D263" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A264" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C264" s="1">
+        <v>121795</v>
+      </c>
+      <c r="D264" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A265" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C265" s="1">
+        <v>121795</v>
+      </c>
+      <c r="D265" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A266" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C266" s="1">
+        <v>121795</v>
+      </c>
+      <c r="D266" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A267" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C267" s="1">
+        <v>121795</v>
+      </c>
+      <c r="D267" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A268" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C268" s="1">
+        <v>121795</v>
+      </c>
+      <c r="D268" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A269" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C269" s="1">
+        <v>121795</v>
+      </c>
+      <c r="D269" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A270" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C270" s="1">
+        <v>121795</v>
+      </c>
+      <c r="D270" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A272" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C272" s="1">
+        <v>1795</v>
+      </c>
+      <c r="D272" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A273" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C273" s="1">
+        <v>1795</v>
+      </c>
+      <c r="D273" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A274" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C274" s="1">
+        <v>1795</v>
+      </c>
+      <c r="D274" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A275" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C275" s="1">
+        <v>1795</v>
+      </c>
+      <c r="D275" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A277" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C277" s="1">
+        <v>21795</v>
+      </c>
+      <c r="D277" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A278" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C278" s="1">
+        <v>21795</v>
+      </c>
+      <c r="D278" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A279" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C279" s="1">
+        <v>21795</v>
+      </c>
+      <c r="D279" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A281" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C281" s="1">
+        <v>181795</v>
+      </c>
+      <c r="D281" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A282" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C282" s="1">
+        <v>181795</v>
+      </c>
+      <c r="D282" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A283" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C283" s="1">
+        <v>181795</v>
+      </c>
+      <c r="D283" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature: plot arbitrary number of conditions
</commit_message>
<xml_diff>
--- a/3D networks data.xlsx
+++ b/3D networks data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nivieru\Documents\MATLAB\Maya code GUI - Niv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20553803-4206-4752-8F5B-A6430A47B887}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EFBE5F-1319-406F-B3F7-20510482B024}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19183" windowHeight="7037" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="342">
   <si>
     <t>Date</t>
   </si>
@@ -930,45 +930,12 @@
     <t>Rambam 10 95% 13mM Mg no EGTA</t>
   </si>
   <si>
-    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix1 95% rambam10 with 13mM Mg\63x\Capture 5</t>
-  </si>
-  <si>
-    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix1 95% rambam10 with 13mM Mg\63x\Capture 6</t>
-  </si>
-  <si>
-    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix1 95% rambam10 with 13mM Mg\63x\Capture 7</t>
-  </si>
-  <si>
-    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix1 95% rambam10 with 13mM Mg\63x\Capture 12</t>
-  </si>
-  <si>
-    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix3 95% rambam10 with 7mM Mg\63x\Capture 4</t>
-  </si>
-  <si>
-    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix3 95% rambam10 with 7mM Mg\63x\Capture 5</t>
-  </si>
-  <si>
-    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix3 95% rambam10 with 7mM Mg\63x\Capture 6</t>
-  </si>
-  <si>
-    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix3 95% rambam10 with 7mM Mg\63x\Capture 8</t>
-  </si>
-  <si>
     <t>Rambam 10 95% 7mM Mg no EGTA</t>
   </si>
   <si>
     <t>Rambam 10 95% 26mM Mg no EGTA</t>
   </si>
   <si>
-    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix2 95% rambam10 with 26mM Mg\63x\Capture 4</t>
-  </si>
-  <si>
-    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix2 95% rambam10 with 26mM Mg\63x\Capture 5</t>
-  </si>
-  <si>
-    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17\mix2 95% rambam10 with 26mM Mg\63x\Capture 7</t>
-  </si>
-  <si>
     <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix1 95% rambam10 with 300nM calyculin sample1\63x\Capture 5</t>
   </si>
   <si>
@@ -1012,6 +979,78 @@
   </si>
   <si>
     <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix1 95% rambam10 with 300nM calyculin sample2\63x\Capture 11</t>
+  </si>
+  <si>
+    <t>Rambam 10 95% 300nM calyculin and 13mM Mg no EGTA</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix2 95% rambam10 with 300nM calyculin and 13mM Mg sample1\63x\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix2 95% rambam10 with 300nM calyculin and 13mM Mg sample1\63x\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix2 95% rambam10 with 300nM calyculin and 13mM Mg sample1\63x\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix2 95% rambam10 with 300nM calyculin and 13mM Mg sample1\63x\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix2 95% rambam10 with 300nM calyculin and 13mM Mg sample1\63x\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix2 95% rambam10 with 300nM calyculin and 13mM Mg sample2\63x\Capture 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix2 95% rambam10 with 300nM calyculin and 13mM Mg sample2\63x\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix2 95% rambam10 with 300nM calyculin and 13mM Mg sample2\63x\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix2 95% rambam10 with 300nM calyculin and 13mM Mg sample2\63x\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix2 95% rambam10 with 300nM calyculin and 13mM Mg sample2\63x\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix2 95% rambam10 with 300nM calyculin and 13mM Mg sample2\63x\Capture 9</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_19 Mg and Calyculin\mix2 95% rambam10 with 300nM calyculin and 13mM Mg sample2\63x\Capture 10</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17 Mg\mix2 95% rambam10 with 26mM Mg\63x\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17 Mg\mix2 95% rambam10 with 26mM Mg\63x\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17 Mg\mix2 95% rambam10 with 26mM Mg\63x\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17 Mg\mix3 95% rambam10 with 7mM Mg\63x\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17 Mg\mix3 95% rambam10 with 7mM Mg\63x\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17 Mg\mix3 95% rambam10 with 7mM Mg\63x\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17 Mg\mix3 95% rambam10 with 7mM Mg\63x\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17 Mg\mix1 95% rambam10 with 13mM Mg\63x\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17 Mg\mix1 95% rambam10 with 13mM Mg\63x\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17 Mg\mix1 95% rambam10 with 13mM Mg\63x\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17 Mg\mix1 95% rambam10 with 13mM Mg\63x\Capture 12</t>
   </si>
 </sst>
 </file>
@@ -1363,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="B219" sqref="B219"/>
+    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
+      <selection activeCell="D231" sqref="D231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4508,7 +4547,7 @@
         <v>131095</v>
       </c>
       <c r="D221" t="s">
-        <v>301</v>
+        <v>338</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.4">
@@ -4522,7 +4561,7 @@
         <v>131095</v>
       </c>
       <c r="D222" t="s">
-        <v>302</v>
+        <v>339</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.4">
@@ -4536,7 +4575,7 @@
         <v>131095</v>
       </c>
       <c r="D223" t="s">
-        <v>303</v>
+        <v>340</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.4">
@@ -4550,7 +4589,7 @@
         <v>131095</v>
       </c>
       <c r="D224" t="s">
-        <v>304</v>
+        <v>341</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.4">
@@ -4558,13 +4597,13 @@
         <v>299</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="C226" s="1">
         <v>71095</v>
       </c>
       <c r="D226" t="s">
-        <v>305</v>
+        <v>334</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.4">
@@ -4572,13 +4611,13 @@
         <v>299</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="C227" s="1">
         <v>71095</v>
       </c>
       <c r="D227" t="s">
-        <v>306</v>
+        <v>336</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.4">
@@ -4586,13 +4625,13 @@
         <v>299</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="C228" s="1">
         <v>71095</v>
       </c>
       <c r="D228" t="s">
-        <v>307</v>
+        <v>335</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.4">
@@ -4600,13 +4639,13 @@
         <v>299</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="C229" s="1">
         <v>71095</v>
       </c>
       <c r="D229" t="s">
-        <v>308</v>
+        <v>337</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.4">
@@ -4614,13 +4653,13 @@
         <v>299</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="C231" s="1">
         <v>261095</v>
       </c>
       <c r="D231" t="s">
-        <v>311</v>
+        <v>331</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.4">
@@ -4628,13 +4667,13 @@
         <v>299</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="C232" s="1">
         <v>261095</v>
       </c>
       <c r="D232" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.4">
@@ -4642,13 +4681,13 @@
         <v>299</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="C233" s="1">
         <v>261095</v>
       </c>
       <c r="D233" t="s">
-        <v>313</v>
+        <v>333</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.4">
@@ -4658,184 +4697,184 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A235" s="5" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C235" s="1">
         <v>3001095</v>
       </c>
       <c r="D235" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A236" s="5" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C236" s="1">
         <v>3001095</v>
       </c>
       <c r="D236" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A237" s="5" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C237" s="1">
         <v>3001095</v>
       </c>
       <c r="D237" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A238" s="5" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C238" s="1">
         <v>3001095</v>
       </c>
       <c r="D238" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A239" s="5" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C239" s="1">
         <v>3001095</v>
       </c>
       <c r="D239" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A240" s="5" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C240" s="1">
         <v>3001095</v>
       </c>
       <c r="D240" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A241" s="5" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C241" s="1">
         <v>3001095</v>
       </c>
       <c r="D241" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A242" s="5" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C242" s="1">
         <v>3001095</v>
       </c>
       <c r="D242" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A243" s="5" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C243" s="1">
         <v>3001095</v>
       </c>
       <c r="D243" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A244" s="5" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C244" s="1">
         <v>3001095</v>
       </c>
       <c r="D244" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A245" s="5" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C245" s="1">
         <v>3001095</v>
       </c>
       <c r="D245" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A246" s="5" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C246" s="1">
         <v>3001095</v>
       </c>
       <c r="D246" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A247" s="5" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C247" s="1">
         <v>3001095</v>
       </c>
       <c r="D247" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.4">
@@ -4844,64 +4883,172 @@
       <c r="C248" s="1"/>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A249" s="5"/>
-      <c r="B249" s="1"/>
-      <c r="C249" s="1"/>
+      <c r="A249" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C249" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D249" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A250" s="5"/>
-      <c r="B250" s="1"/>
-      <c r="C250" s="1"/>
+      <c r="A250" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B250" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C250" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D250" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A251" s="5"/>
-      <c r="B251" s="1"/>
-      <c r="C251" s="1"/>
+      <c r="A251" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C251" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D251" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A252" s="5"/>
-      <c r="B252" s="1"/>
-      <c r="C252" s="1"/>
+      <c r="A252" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B252" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C252" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D252" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A253" s="5"/>
-      <c r="B253" s="1"/>
-      <c r="C253" s="1"/>
+      <c r="A253" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C253" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D253" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A254" s="5"/>
-      <c r="B254" s="1"/>
-      <c r="C254" s="1"/>
+      <c r="A254" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C254" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D254" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A255" s="5"/>
-      <c r="B255" s="1"/>
-      <c r="C255" s="1"/>
+      <c r="A255" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C255" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D255" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A256" s="5"/>
-      <c r="B256" s="1"/>
-      <c r="C256" s="1"/>
+      <c r="A256" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C256" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D256" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A257" s="5"/>
-      <c r="B257" s="1"/>
-      <c r="C257" s="1"/>
+      <c r="A257" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C257" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D257" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A258" s="5"/>
-      <c r="B258" s="1"/>
-      <c r="C258" s="1"/>
+      <c r="A258" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B258" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C258" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D258" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A259" s="5"/>
-      <c r="B259" s="1"/>
-      <c r="C259" s="1"/>
+      <c r="A259" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C259" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D259" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A260" s="5"/>
-      <c r="B260" s="1"/>
-      <c r="C260" s="1"/>
+      <c r="A260" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C260" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D260" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A262" s="5">

</xml_diff>

<commit_message>
a bit restructuring and messeges to the user
</commit_message>
<xml_diff>
--- a/3D networks data.xlsx
+++ b/3D networks data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nivieru\Documents\MATLAB\Maya code GUI - Niv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EFBE5F-1319-406F-B3F7-20510482B024}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF9C079-7342-417D-9CF1-14CE37DDEC07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19183" windowHeight="7037" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="376">
   <si>
     <t>Date</t>
   </si>
@@ -924,9 +924,6 @@
     <t>W:\phkinnerets\storage\analysis\Niv\Rambam17\95% with DDW at 18 degrees\2020_11_11 mix4\63x\Capture 6</t>
   </si>
   <si>
-    <t>11-17-2020</t>
-  </si>
-  <si>
     <t>Rambam 10 95% 13mM Mg no EGTA</t>
   </si>
   <si>
@@ -1051,6 +1048,111 @@
   </si>
   <si>
     <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_17 Mg\mix1 95% rambam10 with 13mM Mg\63x\Capture 12</t>
+  </si>
+  <si>
+    <t>Rambam 10 95% 11mM Mg no EGTA</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix1 95% rambam10 with 11mM Mg sample1\63x\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix1 95% rambam10 with 11mM Mg sample1\63x\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix1 95% rambam10 with 11mM Mg sample1\63x\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix1 95% rambam10 with 11mM Mg sample1\63x\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix1 95% rambam10 with 11mM Mg sample1\63x\Capture 9</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix1 95% rambam10 with 11mM Mg sample2\63x\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix1 95% rambam10 with 11mM Mg sample2\63x\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix1 95% rambam10 with 11mM Mg sample2\63x\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix1 95% rambam10 with 11mM Mg sample2\63x\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix1 95% rambam10 with 11mM Mg sample2\63x\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix1 95% rambam10 with 11mM Mg sample2\63x\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix1 95% rambam10 with 11mM Mg sample2\63x\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix1 95% rambam10 with 11mM Mg sample2\63x\Capture 9</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix1 95% rambam10 with 11mM Mg sample2\63x\Capture 10</t>
+  </si>
+  <si>
+    <t>Rambam 10 95% 9mM Mg no EGTA</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix2 95% rambam10 with 9mM Mg sample1\63x\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix2 95% rambam10 with 9mM Mg sample1\63x\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix2 95% rambam10 with 9mM Mg sample1\63x\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix2 95% rambam10 with 9mM Mg sample1\63x\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix2 95% rambam10 with 9mM Mg sample1\63x\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix2 95% rambam10 with 9mM Mg sample1\63x\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix2 95% rambam10 with 9mM Mg sample1\63x\Capture 9</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix2 95% rambam10 with 9mM Mg sample1\63x\Capture 10</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix2 95% rambam10 with 9mM Mg sample1\63x\Capture 11</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix2 95% rambam10 with 9mM Mg sample1\63x\Capture 12</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix2 95% rambam10 with 9mM Mg sample2\63x\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix2 95% rambam10 with 9mM Mg sample2\63x\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix2 95% rambam10 with 9mM Mg sample2\63x\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix2 95% rambam10 with 9mM Mg sample2\63x\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix2 95% rambam10 with 9mM Mg sample2\63x\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix2 95% rambam10 with 9mM Mg sample2\63x\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix2 95% rambam10 with 9mM Mg sample2\63x\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix2 95% rambam10 with 9mM Mg sample2\63x\Capture 9</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix2 95% rambam10 with 9mM Mg sample2\63x\Capture 10</t>
   </si>
 </sst>
 </file>
@@ -1400,10 +1502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BF283"/>
+  <dimension ref="A1:BF326"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
-      <selection activeCell="D231" sqref="D231"/>
+    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
+      <selection activeCell="C258" sqref="C258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4426,7 +4528,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A212" s="5">
-        <v>44054</v>
+        <v>44143</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>268</v>
@@ -4440,7 +4542,7 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A213" s="5">
-        <v>44054</v>
+        <v>44143</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>268</v>
@@ -4454,7 +4556,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A214" s="5">
-        <v>44054</v>
+        <v>44143</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>268</v>
@@ -4468,7 +4570,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A215" s="5">
-        <v>44054</v>
+        <v>44143</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>268</v>
@@ -4482,7 +4584,7 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A216" s="5">
-        <v>44054</v>
+        <v>44143</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>268</v>
@@ -4496,7 +4598,7 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A217" s="5">
-        <v>44054</v>
+        <v>44143</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>268</v>
@@ -4510,7 +4612,7 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A218" s="5">
-        <v>44054</v>
+        <v>44143</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>268</v>
@@ -4524,7 +4626,7 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A219" s="5">
-        <v>44054</v>
+        <v>44143</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>268</v>
@@ -4537,157 +4639,157 @@
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A221" s="5" t="s">
+      <c r="A221" s="5">
+        <v>44152</v>
+      </c>
+      <c r="B221" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="B221" s="1" t="s">
-        <v>300</v>
       </c>
       <c r="C221" s="1">
         <v>131095</v>
       </c>
       <c r="D221" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A222" s="5" t="s">
+      <c r="A222" s="5">
+        <v>44152</v>
+      </c>
+      <c r="B222" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="B222" s="1" t="s">
-        <v>300</v>
       </c>
       <c r="C222" s="1">
         <v>131095</v>
       </c>
       <c r="D222" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A223" s="5" t="s">
+      <c r="A223" s="5">
+        <v>44152</v>
+      </c>
+      <c r="B223" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="B223" s="1" t="s">
-        <v>300</v>
       </c>
       <c r="C223" s="1">
         <v>131095</v>
       </c>
       <c r="D223" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A224" s="5" t="s">
+      <c r="A224" s="5">
+        <v>44152</v>
+      </c>
+      <c r="B224" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="B224" s="1" t="s">
-        <v>300</v>
       </c>
       <c r="C224" s="1">
         <v>131095</v>
       </c>
       <c r="D224" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A226" s="5" t="s">
-        <v>299</v>
+      <c r="A226" s="5">
+        <v>44152</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C226" s="1">
         <v>71095</v>
       </c>
       <c r="D226" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A227" s="5" t="s">
-        <v>299</v>
+      <c r="A227" s="5">
+        <v>44152</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C227" s="1">
         <v>71095</v>
       </c>
       <c r="D227" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A228" s="5" t="s">
-        <v>299</v>
+      <c r="A228" s="5">
+        <v>44152</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C228" s="1">
         <v>71095</v>
       </c>
       <c r="D228" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A229" s="5" t="s">
-        <v>299</v>
+      <c r="A229" s="5">
+        <v>44152</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C229" s="1">
         <v>71095</v>
       </c>
       <c r="D229" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A231" s="5" t="s">
-        <v>299</v>
+      <c r="A231" s="5">
+        <v>44152</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C231" s="1">
         <v>261095</v>
       </c>
       <c r="D231" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A232" s="5" t="s">
-        <v>299</v>
+      <c r="A232" s="5">
+        <v>44152</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C232" s="1">
         <v>261095</v>
       </c>
       <c r="D232" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A233" s="5" t="s">
-        <v>299</v>
+      <c r="A233" s="5">
+        <v>44152</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C233" s="1">
         <v>261095</v>
       </c>
       <c r="D233" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.4">
@@ -4696,623 +4798,1135 @@
       <c r="C234" s="1"/>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A235" s="5" t="s">
-        <v>305</v>
+      <c r="A235" s="5">
+        <v>44160</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>304</v>
+        <v>341</v>
       </c>
       <c r="C235" s="1">
-        <v>3001095</v>
+        <v>111095</v>
       </c>
       <c r="D235" t="s">
-        <v>303</v>
+        <v>342</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A236" s="5" t="s">
-        <v>305</v>
+      <c r="A236" s="5">
+        <v>44160</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>304</v>
+        <v>341</v>
       </c>
       <c r="C236" s="1">
-        <v>3001095</v>
+        <v>111095</v>
       </c>
       <c r="D236" t="s">
-        <v>306</v>
+        <v>343</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A237" s="5" t="s">
-        <v>305</v>
+      <c r="A237" s="5">
+        <v>44160</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>304</v>
+        <v>341</v>
       </c>
       <c r="C237" s="1">
-        <v>3001095</v>
+        <v>111095</v>
       </c>
       <c r="D237" t="s">
-        <v>307</v>
+        <v>344</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A238" s="5" t="s">
-        <v>305</v>
+      <c r="A238" s="5">
+        <v>44160</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>304</v>
+        <v>341</v>
       </c>
       <c r="C238" s="1">
-        <v>3001095</v>
+        <v>111095</v>
       </c>
       <c r="D238" t="s">
-        <v>308</v>
+        <v>345</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A239" s="5" t="s">
-        <v>305</v>
+      <c r="A239" s="5">
+        <v>44160</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>304</v>
+        <v>341</v>
       </c>
       <c r="C239" s="1">
-        <v>3001095</v>
+        <v>111095</v>
       </c>
       <c r="D239" t="s">
-        <v>309</v>
+        <v>346</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A240" s="5" t="s">
-        <v>305</v>
+      <c r="A240" s="5">
+        <v>44160</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>304</v>
+        <v>341</v>
       </c>
       <c r="C240" s="1">
-        <v>3001095</v>
+        <v>111095</v>
       </c>
       <c r="D240" t="s">
-        <v>310</v>
+        <v>347</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A241" s="5" t="s">
-        <v>305</v>
+      <c r="A241" s="5">
+        <v>44160</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>304</v>
+        <v>341</v>
       </c>
       <c r="C241" s="1">
-        <v>3001095</v>
+        <v>111095</v>
       </c>
       <c r="D241" t="s">
-        <v>311</v>
+        <v>348</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A242" s="5" t="s">
-        <v>305</v>
+      <c r="A242" s="5">
+        <v>44160</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>304</v>
+        <v>341</v>
       </c>
       <c r="C242" s="1">
-        <v>3001095</v>
+        <v>111095</v>
       </c>
       <c r="D242" t="s">
-        <v>312</v>
+        <v>349</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A243" s="5" t="s">
-        <v>305</v>
+      <c r="A243" s="5">
+        <v>44160</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>304</v>
+        <v>341</v>
       </c>
       <c r="C243" s="1">
-        <v>3001095</v>
+        <v>111095</v>
       </c>
       <c r="D243" t="s">
-        <v>313</v>
+        <v>350</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A244" s="5" t="s">
-        <v>305</v>
+      <c r="A244" s="5">
+        <v>44160</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>304</v>
+        <v>341</v>
       </c>
       <c r="C244" s="1">
-        <v>3001095</v>
+        <v>111095</v>
       </c>
       <c r="D244" t="s">
-        <v>314</v>
+        <v>351</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A245" s="5" t="s">
-        <v>305</v>
+      <c r="A245" s="5">
+        <v>44160</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>304</v>
+        <v>341</v>
       </c>
       <c r="C245" s="1">
-        <v>3001095</v>
+        <v>111095</v>
       </c>
       <c r="D245" t="s">
-        <v>315</v>
+        <v>352</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A246" s="5" t="s">
-        <v>305</v>
+      <c r="A246" s="5">
+        <v>44160</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>304</v>
+        <v>341</v>
       </c>
       <c r="C246" s="1">
-        <v>3001095</v>
+        <v>111095</v>
       </c>
       <c r="D246" t="s">
-        <v>316</v>
+        <v>353</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A247" s="5" t="s">
-        <v>305</v>
+      <c r="A247" s="5">
+        <v>44160</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>304</v>
+        <v>341</v>
       </c>
       <c r="C247" s="1">
-        <v>3001095</v>
+        <v>111095</v>
       </c>
       <c r="D247" t="s">
-        <v>317</v>
+        <v>354</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A248" s="5"/>
-      <c r="B248" s="1"/>
-      <c r="C248" s="1"/>
+      <c r="A248" s="5">
+        <v>44160</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C248" s="1">
+        <v>111095</v>
+      </c>
+      <c r="D248" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A249" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="B249" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="C249" s="1">
-        <v>300131095</v>
-      </c>
-      <c r="D249" t="s">
-        <v>319</v>
-      </c>
+      <c r="A249" s="5"/>
+      <c r="B249" s="1"/>
+      <c r="C249" s="1"/>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A250" s="5" t="s">
-        <v>305</v>
+      <c r="A250" s="5">
+        <v>44160</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>318</v>
+        <v>356</v>
       </c>
       <c r="C250" s="1">
-        <v>300131095</v>
+        <v>91095</v>
       </c>
       <c r="D250" t="s">
-        <v>320</v>
+        <v>357</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A251" s="5" t="s">
-        <v>305</v>
+      <c r="A251" s="5">
+        <v>44160</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>318</v>
+        <v>356</v>
       </c>
       <c r="C251" s="1">
-        <v>300131095</v>
+        <v>91095</v>
       </c>
       <c r="D251" t="s">
-        <v>321</v>
+        <v>358</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A252" s="5" t="s">
-        <v>305</v>
+      <c r="A252" s="5">
+        <v>44160</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>318</v>
+        <v>356</v>
       </c>
       <c r="C252" s="1">
-        <v>300131095</v>
+        <v>91095</v>
       </c>
       <c r="D252" t="s">
-        <v>322</v>
+        <v>359</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A253" s="5" t="s">
-        <v>305</v>
+      <c r="A253" s="5">
+        <v>44160</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>318</v>
+        <v>356</v>
       </c>
       <c r="C253" s="1">
-        <v>300131095</v>
+        <v>91095</v>
       </c>
       <c r="D253" t="s">
-        <v>323</v>
+        <v>360</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A254" s="5" t="s">
-        <v>305</v>
+      <c r="A254" s="5">
+        <v>44160</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>318</v>
+        <v>356</v>
       </c>
       <c r="C254" s="1">
-        <v>300131095</v>
+        <v>91095</v>
       </c>
       <c r="D254" t="s">
-        <v>324</v>
+        <v>361</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A255" s="5" t="s">
-        <v>305</v>
+      <c r="A255" s="5">
+        <v>44160</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>318</v>
+        <v>356</v>
       </c>
       <c r="C255" s="1">
-        <v>300131095</v>
+        <v>91095</v>
       </c>
       <c r="D255" t="s">
-        <v>325</v>
+        <v>362</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A256" s="5" t="s">
-        <v>305</v>
+      <c r="A256" s="5">
+        <v>44160</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>318</v>
+        <v>356</v>
       </c>
       <c r="C256" s="1">
-        <v>300131095</v>
+        <v>91095</v>
       </c>
       <c r="D256" t="s">
-        <v>326</v>
+        <v>363</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A257" s="5" t="s">
-        <v>305</v>
+      <c r="A257" s="5">
+        <v>44160</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>318</v>
+        <v>356</v>
       </c>
       <c r="C257" s="1">
-        <v>300131095</v>
+        <v>91095</v>
       </c>
       <c r="D257" t="s">
-        <v>327</v>
+        <v>364</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A258" s="5" t="s">
-        <v>305</v>
+      <c r="A258" s="5">
+        <v>44160</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>318</v>
+        <v>356</v>
       </c>
       <c r="C258" s="1">
-        <v>300131095</v>
+        <v>91095</v>
       </c>
       <c r="D258" t="s">
-        <v>328</v>
+        <v>365</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A259" s="5" t="s">
-        <v>305</v>
+      <c r="A259" s="5">
+        <v>44160</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>318</v>
+        <v>356</v>
       </c>
       <c r="C259" s="1">
-        <v>300131095</v>
+        <v>91095</v>
       </c>
       <c r="D259" t="s">
-        <v>329</v>
+        <v>366</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A260" s="5" t="s">
-        <v>305</v>
+      <c r="A260" s="5">
+        <v>44160</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>318</v>
+        <v>356</v>
       </c>
       <c r="C260" s="1">
-        <v>300131095</v>
+        <v>91095</v>
       </c>
       <c r="D260" t="s">
-        <v>330</v>
+        <v>367</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A261" s="5">
+        <v>44160</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C261" s="1">
+        <v>91095</v>
+      </c>
+      <c r="D261" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A262" s="5">
-        <v>44146</v>
+        <v>44160</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>276</v>
+        <v>356</v>
       </c>
       <c r="C262" s="1">
-        <v>121795</v>
+        <v>91095</v>
       </c>
       <c r="D262" t="s">
-        <v>277</v>
+        <v>369</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A263" s="5">
-        <v>44146</v>
+        <v>44160</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>276</v>
+        <v>356</v>
       </c>
       <c r="C263" s="1">
-        <v>121795</v>
+        <v>91095</v>
       </c>
       <c r="D263" t="s">
-        <v>278</v>
+        <v>370</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A264" s="5">
-        <v>44146</v>
+        <v>44160</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>276</v>
+        <v>356</v>
       </c>
       <c r="C264" s="1">
-        <v>121795</v>
+        <v>91095</v>
       </c>
       <c r="D264" t="s">
-        <v>279</v>
+        <v>371</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A265" s="5">
-        <v>44146</v>
+        <v>44160</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>276</v>
+        <v>356</v>
       </c>
       <c r="C265" s="1">
-        <v>121795</v>
+        <v>91095</v>
       </c>
       <c r="D265" t="s">
-        <v>280</v>
+        <v>372</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A266" s="5">
-        <v>44146</v>
+        <v>44160</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>276</v>
+        <v>356</v>
       </c>
       <c r="C266" s="1">
-        <v>121795</v>
+        <v>91095</v>
       </c>
       <c r="D266" t="s">
-        <v>281</v>
+        <v>373</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A267" s="5">
-        <v>44146</v>
+        <v>44160</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>276</v>
+        <v>356</v>
       </c>
       <c r="C267" s="1">
-        <v>121795</v>
+        <v>91095</v>
       </c>
       <c r="D267" t="s">
-        <v>282</v>
+        <v>374</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A268" s="5">
+        <v>44160</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C268" s="1">
+        <v>91095</v>
+      </c>
+      <c r="D268" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A269" s="5"/>
+      <c r="B269" s="1"/>
+      <c r="C269" s="1"/>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A270" s="5"/>
+      <c r="B270" s="1"/>
+      <c r="C270" s="1"/>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A271" s="5"/>
+      <c r="B271" s="1"/>
+      <c r="C271" s="1"/>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A272" s="5"/>
+      <c r="B272" s="1"/>
+      <c r="C272" s="1"/>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A273" s="5"/>
+      <c r="B273" s="1"/>
+      <c r="C273" s="1"/>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A274" s="5"/>
+      <c r="B274" s="1"/>
+      <c r="C274" s="1"/>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A275" s="5"/>
+      <c r="B275" s="1"/>
+      <c r="C275" s="1"/>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A276" s="5"/>
+      <c r="B276" s="1"/>
+      <c r="C276" s="1"/>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A277" s="5"/>
+      <c r="B277" s="1"/>
+      <c r="C277" s="1"/>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A278" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C278" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D278" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A279" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C279" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D279" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A280" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C280" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D280" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A281" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C281" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D281" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A282" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C282" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D282" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A283" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C283" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D283" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A284" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C284" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D284" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A285" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C285" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D285" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A286" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C286" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D286" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A287" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C287" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D287" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A288" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C288" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D288" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A289" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C289" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D289" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A290" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C290" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D290" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A291" s="5"/>
+      <c r="B291" s="1"/>
+      <c r="C291" s="1"/>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A292" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C292" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D292" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A293" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C293" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D293" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A294" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C294" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D294" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A295" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B295" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C295" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D295" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A296" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C296" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D296" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A297" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B297" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C297" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D297" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A298" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B298" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C298" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D298" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A299" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B299" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C299" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D299" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A300" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B300" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C300" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D300" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A301" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B301" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C301" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D301" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A302" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B302" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C302" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D302" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A303" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C303" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D303" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A305" s="5">
         <v>44146</v>
       </c>
-      <c r="B268" s="1" t="s">
+      <c r="B305" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C268" s="1">
+      <c r="C305" s="1">
         <v>121795</v>
       </c>
-      <c r="D268" t="s">
+      <c r="D305" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A306" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B306" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C306" s="1">
+        <v>121795</v>
+      </c>
+      <c r="D306" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A307" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C307" s="1">
+        <v>121795</v>
+      </c>
+      <c r="D307" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A308" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B308" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C308" s="1">
+        <v>121795</v>
+      </c>
+      <c r="D308" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A309" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B309" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C309" s="1">
+        <v>121795</v>
+      </c>
+      <c r="D309" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A310" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C310" s="1">
+        <v>121795</v>
+      </c>
+      <c r="D310" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A311" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B311" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C311" s="1">
+        <v>121795</v>
+      </c>
+      <c r="D311" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A269" s="5">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A312" s="5">
         <v>44146</v>
       </c>
-      <c r="B269" s="1" t="s">
+      <c r="B312" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C269" s="1">
+      <c r="C312" s="1">
         <v>121795</v>
       </c>
-      <c r="D269" t="s">
+      <c r="D312" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A270" s="5">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A313" s="5">
         <v>44146</v>
       </c>
-      <c r="B270" s="1" t="s">
+      <c r="B313" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C270" s="1">
+      <c r="C313" s="1">
         <v>121795</v>
       </c>
-      <c r="D270" t="s">
+      <c r="D313" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A272" s="5">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A315" s="5">
         <v>44146</v>
       </c>
-      <c r="B272" s="1" t="s">
+      <c r="B315" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="C272" s="1">
+      <c r="C315" s="1">
         <v>1795</v>
       </c>
-      <c r="D272" t="s">
+      <c r="D315" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A273" s="5">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A316" s="5">
         <v>44146</v>
       </c>
-      <c r="B273" s="1" t="s">
+      <c r="B316" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="C273" s="1">
+      <c r="C316" s="1">
         <v>1795</v>
       </c>
-      <c r="D273" t="s">
+      <c r="D316" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A274" s="5">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A317" s="5">
         <v>44146</v>
       </c>
-      <c r="B274" s="1" t="s">
+      <c r="B317" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="C274" s="1">
+      <c r="C317" s="1">
         <v>1795</v>
       </c>
-      <c r="D274" t="s">
+      <c r="D317" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A275" s="5">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A318" s="5">
         <v>44146</v>
       </c>
-      <c r="B275" s="1" t="s">
+      <c r="B318" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="C275" s="1">
+      <c r="C318" s="1">
         <v>1795</v>
       </c>
-      <c r="D275" t="s">
+      <c r="D318" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A277" s="5">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A320" s="5">
         <v>44146</v>
       </c>
-      <c r="B277" s="1" t="s">
+      <c r="B320" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C277" s="1">
+      <c r="C320" s="1">
         <v>21795</v>
       </c>
-      <c r="D277" t="s">
+      <c r="D320" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A278" s="5">
+    <row r="321" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A321" s="5">
         <v>44146</v>
       </c>
-      <c r="B278" s="1" t="s">
+      <c r="B321" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C278" s="1">
+      <c r="C321" s="1">
         <v>21795</v>
       </c>
-      <c r="D278" t="s">
+      <c r="D321" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A279" s="5">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A322" s="5">
         <v>44146</v>
       </c>
-      <c r="B279" s="1" t="s">
+      <c r="B322" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C279" s="1">
+      <c r="C322" s="1">
         <v>21795</v>
       </c>
-      <c r="D279" t="s">
+      <c r="D322" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A281" s="5">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A324" s="5">
         <v>44146</v>
       </c>
-      <c r="B281" s="1" t="s">
+      <c r="B324" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="C281" s="1">
+      <c r="C324" s="1">
         <v>181795</v>
       </c>
-      <c r="D281" t="s">
+      <c r="D324" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A282" s="5">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A325" s="5">
         <v>44146</v>
       </c>
-      <c r="B282" s="1" t="s">
+      <c r="B325" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="C282" s="1">
+      <c r="C325" s="1">
         <v>181795</v>
       </c>
-      <c r="D282" t="s">
+      <c r="D325" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A283" s="5">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A326" s="5">
         <v>44146</v>
       </c>
-      <c r="B283" s="1" t="s">
+      <c r="B326" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="C283" s="1">
+      <c r="C326" s="1">
         <v>181795</v>
       </c>
-      <c r="D283" t="s">
+      <c r="D326" t="s">
         <v>298</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new plots ui
</commit_message>
<xml_diff>
--- a/3D networks data.xlsx
+++ b/3D networks data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nivieru\Documents\MATLAB\Maya code GUI - Niv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF9C079-7342-417D-9CF1-14CE37DDEC07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335F552C-5543-4A4D-BA8D-1F189FF18FF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19183" windowHeight="7037" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="415">
   <si>
     <t>Date</t>
   </si>
@@ -1153,6 +1153,123 @@
   </si>
   <si>
     <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_11_25 Mg\mix2 95% rambam10 with 9mM Mg sample2\63x\Capture 10</t>
+  </si>
+  <si>
+    <t>Rambam 10 95% 30deg</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix1 rambam10 95% sample1 30deg\Capture 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix1 rambam10 95% sample1 30deg\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix1 rambam10 95% sample1 30deg\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix1 rambam10 95% sample1 30deg\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix1 rambam10 95% sample1 30deg\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix1 rambam10 95% sample1 30deg\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix1 rambam10 95% sample2 30deg\Capture 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix1 rambam10 95% sample2 30deg\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix1 rambam10 95% sample2 30deg\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix1 rambam10 95% sample2 30deg\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix1 rambam10 95% sample2 30deg\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix1 rambam10 95% sample2 30deg\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix1 rambam10 95% sample2 30deg\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix2 rambam10 95% sample2 30deg\Capture 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix2 rambam10 95% sample2 30deg\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix2 rambam10 95% sample2 30deg\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix2 rambam10 95% sample2 30deg\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix2 rambam10 95% sample2 30deg\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix2 rambam10 95% sample2 30deg\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix2 rambam10 95% sample2 30deg\Capture 9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rambam 10 95% 30deg 300nM calyculin and 13mM Mg </t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_07 temperature, Mg, and Calyculin\mix1 95% rambam10 with 300nm calyculin A and 13mM Mg sample1 30deg\63x\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_07 temperature, Mg, and Calyculin\mix1 95% rambam10 with 300nm calyculin A and 13mM Mg sample1 30deg\63x\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_07 temperature, Mg, and Calyculin\mix1 95% rambam10 with 300nm calyculin A and 13mM Mg sample1 30deg\63x\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_07 temperature, Mg, and Calyculin\mix1 95% rambam10 with 300nm calyculin A and 13mM Mg sample1 30deg\63x\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_07 temperature, Mg, and Calyculin\mix1 95% rambam10 with 300nm calyculin A and 13mM Mg sample1 30deg\63x\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_07 temperature, Mg, and Calyculin\mix1 95% rambam10 with 300nm calyculin A and 13mM Mg sample1 30deg\63x\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_07 temperature, Mg, and Calyculin\mix1 95% rambam10 with 300nm calyculin A and 13mM Mg sample2 30deg\Capture 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_07 temperature, Mg, and Calyculin\mix1 95% rambam10 with 300nm calyculin A and 13mM Mg sample2 30deg\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_07 temperature, Mg, and Calyculin\mix1 95% rambam10 with 300nm calyculin A and 13mM Mg sample2 30deg\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_07 temperature, Mg, and Calyculin\mix1 95% rambam10 with 300nm calyculin A and 13mM Mg sample2 30deg\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_07 temperature, Mg, and Calyculin\mix1 95% rambam10 with 300nm calyculin A and 13mM Mg sample2 30deg\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix2 rambam10 95% sample1 25deg\Capture 1</t>
+  </si>
+  <si>
+    <t>Rambam 10 95% 25deg</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix2 rambam10 95% sample1 25deg\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix2 rambam10 95% sample1 25deg\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix2 rambam10 95% sample1 25deg\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix2 rambam10 95% sample1 25deg\Capture 5</t>
   </si>
 </sst>
 </file>
@@ -1502,10 +1619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BF326"/>
+  <dimension ref="A1:BF357"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="C258" sqref="C258"/>
+    <sheetView tabSelected="1" topLeftCell="A324" workbookViewId="0">
+      <selection activeCell="C291" sqref="C291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -5270,663 +5387,1137 @@
       <c r="C269" s="1"/>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A270" s="5"/>
-      <c r="B270" s="1"/>
-      <c r="C270" s="1"/>
+      <c r="A270" s="5">
+        <v>44171</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C270" s="1">
+        <v>301095</v>
+      </c>
+      <c r="D270" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A271" s="5"/>
-      <c r="B271" s="1"/>
-      <c r="C271" s="1"/>
+      <c r="A271" s="5">
+        <v>44171</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C271" s="1">
+        <v>301095</v>
+      </c>
+      <c r="D271" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A272" s="5"/>
-      <c r="B272" s="1"/>
-      <c r="C272" s="1"/>
+      <c r="A272" s="5">
+        <v>44171</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C272" s="1">
+        <v>301095</v>
+      </c>
+      <c r="D272" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A273" s="5"/>
-      <c r="B273" s="1"/>
-      <c r="C273" s="1"/>
+      <c r="A273" s="5">
+        <v>44171</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C273" s="1">
+        <v>301095</v>
+      </c>
+      <c r="D273" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A274" s="5"/>
-      <c r="B274" s="1"/>
-      <c r="C274" s="1"/>
+      <c r="A274" s="5">
+        <v>44171</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C274" s="1">
+        <v>301095</v>
+      </c>
+      <c r="D274" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A275" s="5"/>
-      <c r="B275" s="1"/>
-      <c r="C275" s="1"/>
+      <c r="A275" s="5">
+        <v>44171</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C275" s="1">
+        <v>301095</v>
+      </c>
+      <c r="D275" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A276" s="5"/>
-      <c r="B276" s="1"/>
-      <c r="C276" s="1"/>
+      <c r="A276" s="5">
+        <v>44171</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C276" s="1">
+        <v>301095</v>
+      </c>
+      <c r="D276" t="s">
+        <v>383</v>
+      </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A277" s="5"/>
-      <c r="B277" s="1"/>
-      <c r="C277" s="1"/>
+      <c r="A277" s="5">
+        <v>44171</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C277" s="1">
+        <v>301095</v>
+      </c>
+      <c r="D277" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A278" s="5" t="s">
-        <v>304</v>
+      <c r="A278" s="5">
+        <v>44171</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>303</v>
+        <v>376</v>
       </c>
       <c r="C278" s="1">
-        <v>3001095</v>
+        <v>301095</v>
       </c>
       <c r="D278" t="s">
-        <v>302</v>
+        <v>385</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A279" s="5" t="s">
-        <v>304</v>
+      <c r="A279" s="5">
+        <v>44171</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>303</v>
+        <v>376</v>
       </c>
       <c r="C279" s="1">
-        <v>3001095</v>
+        <v>301095</v>
       </c>
       <c r="D279" t="s">
-        <v>305</v>
+        <v>386</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A280" s="5" t="s">
-        <v>304</v>
+      <c r="A280" s="5">
+        <v>44171</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>303</v>
+        <v>376</v>
       </c>
       <c r="C280" s="1">
-        <v>3001095</v>
+        <v>301095</v>
       </c>
       <c r="D280" t="s">
-        <v>306</v>
+        <v>387</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A281" s="5" t="s">
-        <v>304</v>
+      <c r="A281" s="5">
+        <v>44171</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>303</v>
+        <v>376</v>
       </c>
       <c r="C281" s="1">
-        <v>3001095</v>
+        <v>301095</v>
       </c>
       <c r="D281" t="s">
-        <v>307</v>
+        <v>388</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A282" s="5" t="s">
-        <v>304</v>
+      <c r="A282" s="5">
+        <v>44171</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>303</v>
+        <v>376</v>
       </c>
       <c r="C282" s="1">
-        <v>3001095</v>
+        <v>301095</v>
       </c>
       <c r="D282" t="s">
-        <v>308</v>
+        <v>389</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A283" s="5" t="s">
-        <v>304</v>
+      <c r="A283" s="5">
+        <v>44171</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>303</v>
+        <v>376</v>
       </c>
       <c r="C283" s="1">
-        <v>3001095</v>
+        <v>301095</v>
       </c>
       <c r="D283" t="s">
-        <v>309</v>
+        <v>390</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A284" s="5" t="s">
-        <v>304</v>
+      <c r="A284" s="5">
+        <v>44171</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>303</v>
+        <v>376</v>
       </c>
       <c r="C284" s="1">
-        <v>3001095</v>
+        <v>301095</v>
       </c>
       <c r="D284" t="s">
-        <v>310</v>
+        <v>391</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A285" s="5" t="s">
-        <v>304</v>
+      <c r="A285" s="5">
+        <v>44171</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>303</v>
+        <v>376</v>
       </c>
       <c r="C285" s="1">
-        <v>3001095</v>
+        <v>301095</v>
       </c>
       <c r="D285" t="s">
-        <v>311</v>
+        <v>392</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A286" s="5" t="s">
-        <v>304</v>
+      <c r="A286" s="5">
+        <v>44171</v>
       </c>
       <c r="B286" s="1" t="s">
-        <v>303</v>
+        <v>376</v>
       </c>
       <c r="C286" s="1">
-        <v>3001095</v>
+        <v>301095</v>
       </c>
       <c r="D286" t="s">
-        <v>312</v>
+        <v>393</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A287" s="5" t="s">
-        <v>304</v>
+      <c r="A287" s="5">
+        <v>44171</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>303</v>
+        <v>376</v>
       </c>
       <c r="C287" s="1">
-        <v>3001095</v>
+        <v>301095</v>
       </c>
       <c r="D287" t="s">
-        <v>313</v>
+        <v>394</v>
       </c>
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A288" s="5" t="s">
-        <v>304</v>
+      <c r="A288" s="5">
+        <v>44171</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>303</v>
+        <v>376</v>
       </c>
       <c r="C288" s="1">
-        <v>3001095</v>
+        <v>301095</v>
       </c>
       <c r="D288" t="s">
-        <v>314</v>
+        <v>395</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A289" s="5" t="s">
-        <v>304</v>
+      <c r="A289" s="5">
+        <v>44171</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>303</v>
+        <v>376</v>
       </c>
       <c r="C289" s="1">
-        <v>3001095</v>
+        <v>301095</v>
       </c>
       <c r="D289" t="s">
-        <v>315</v>
+        <v>396</v>
       </c>
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A290" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="B290" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="C290" s="1">
-        <v>3001095</v>
-      </c>
-      <c r="D290" t="s">
-        <v>316</v>
-      </c>
+      <c r="A290" s="5"/>
+      <c r="B290" s="1"/>
+      <c r="C290" s="1"/>
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A291" s="5"/>
-      <c r="B291" s="1"/>
-      <c r="C291" s="1"/>
+      <c r="A291" s="5">
+        <v>44171</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C291" s="1">
+        <v>251095</v>
+      </c>
+      <c r="D291" t="s">
+        <v>409</v>
+      </c>
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A292" s="5" t="s">
-        <v>304</v>
+      <c r="A292" s="5">
+        <v>44171</v>
       </c>
       <c r="B292" s="1" t="s">
-        <v>317</v>
+        <v>410</v>
       </c>
       <c r="C292" s="1">
-        <v>300131095</v>
+        <v>251095</v>
       </c>
       <c r="D292" t="s">
-        <v>318</v>
+        <v>411</v>
       </c>
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A293" s="5" t="s">
-        <v>304</v>
+      <c r="A293" s="5">
+        <v>44171</v>
       </c>
       <c r="B293" s="1" t="s">
-        <v>317</v>
+        <v>410</v>
       </c>
       <c r="C293" s="1">
-        <v>300131095</v>
+        <v>251095</v>
       </c>
       <c r="D293" t="s">
-        <v>319</v>
+        <v>412</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A294" s="5" t="s">
-        <v>304</v>
+      <c r="A294" s="5">
+        <v>44171</v>
       </c>
       <c r="B294" s="1" t="s">
-        <v>317</v>
+        <v>410</v>
       </c>
       <c r="C294" s="1">
-        <v>300131095</v>
+        <v>251095</v>
       </c>
       <c r="D294" t="s">
-        <v>320</v>
+        <v>413</v>
       </c>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A295" s="5" t="s">
-        <v>304</v>
+      <c r="A295" s="5">
+        <v>44171</v>
       </c>
       <c r="B295" s="1" t="s">
-        <v>317</v>
+        <v>410</v>
       </c>
       <c r="C295" s="1">
-        <v>300131095</v>
+        <v>251095</v>
       </c>
       <c r="D295" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A296" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="B296" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="C296" s="1">
-        <v>300131095</v>
-      </c>
-      <c r="D296" t="s">
-        <v>322</v>
+        <v>414</v>
       </c>
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A297" s="5" t="s">
-        <v>304</v>
+      <c r="A297" s="5">
+        <v>44172</v>
       </c>
       <c r="B297" s="1" t="s">
-        <v>317</v>
+        <v>397</v>
       </c>
       <c r="C297" s="1">
-        <v>300131095</v>
+        <v>30300131095</v>
       </c>
       <c r="D297" t="s">
-        <v>323</v>
+        <v>398</v>
       </c>
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A298" s="5" t="s">
-        <v>304</v>
+      <c r="A298" s="5">
+        <v>44172</v>
       </c>
       <c r="B298" s="1" t="s">
-        <v>317</v>
+        <v>397</v>
       </c>
       <c r="C298" s="1">
-        <v>300131095</v>
+        <v>30300131095</v>
       </c>
       <c r="D298" t="s">
-        <v>324</v>
+        <v>399</v>
       </c>
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A299" s="5" t="s">
-        <v>304</v>
+      <c r="A299" s="5">
+        <v>44172</v>
       </c>
       <c r="B299" s="1" t="s">
-        <v>317</v>
+        <v>397</v>
       </c>
       <c r="C299" s="1">
-        <v>300131095</v>
+        <v>30300131095</v>
       </c>
       <c r="D299" t="s">
-        <v>325</v>
+        <v>400</v>
       </c>
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A300" s="5" t="s">
-        <v>304</v>
+      <c r="A300" s="5">
+        <v>44172</v>
       </c>
       <c r="B300" s="1" t="s">
-        <v>317</v>
+        <v>397</v>
       </c>
       <c r="C300" s="1">
-        <v>300131095</v>
+        <v>30300131095</v>
       </c>
       <c r="D300" t="s">
-        <v>326</v>
+        <v>401</v>
       </c>
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A301" s="5" t="s">
-        <v>304</v>
+      <c r="A301" s="5">
+        <v>44172</v>
       </c>
       <c r="B301" s="1" t="s">
-        <v>317</v>
+        <v>397</v>
       </c>
       <c r="C301" s="1">
-        <v>300131095</v>
+        <v>30300131095</v>
       </c>
       <c r="D301" t="s">
-        <v>327</v>
+        <v>402</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A302" s="5" t="s">
-        <v>304</v>
+      <c r="A302" s="5">
+        <v>44172</v>
       </c>
       <c r="B302" s="1" t="s">
-        <v>317</v>
+        <v>397</v>
       </c>
       <c r="C302" s="1">
-        <v>300131095</v>
+        <v>30300131095</v>
       </c>
       <c r="D302" t="s">
-        <v>328</v>
+        <v>403</v>
       </c>
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A303" s="5" t="s">
-        <v>304</v>
+      <c r="A303" s="5">
+        <v>44172</v>
       </c>
       <c r="B303" s="1" t="s">
-        <v>317</v>
+        <v>397</v>
       </c>
       <c r="C303" s="1">
-        <v>300131095</v>
+        <v>30300131095</v>
       </c>
       <c r="D303" t="s">
-        <v>329</v>
+        <v>404</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A304" s="5">
+        <v>44172</v>
+      </c>
+      <c r="B304" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C304" s="1">
+        <v>30300131095</v>
+      </c>
+      <c r="D304" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A305" s="5">
-        <v>44146</v>
+        <v>44172</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>276</v>
+        <v>397</v>
       </c>
       <c r="C305" s="1">
-        <v>121795</v>
+        <v>30300131095</v>
       </c>
       <c r="D305" t="s">
-        <v>277</v>
+        <v>406</v>
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A306" s="5">
-        <v>44146</v>
+        <v>44172</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>276</v>
+        <v>397</v>
       </c>
       <c r="C306" s="1">
-        <v>121795</v>
+        <v>30300131095</v>
       </c>
       <c r="D306" t="s">
-        <v>278</v>
+        <v>407</v>
       </c>
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A307" s="5">
+        <v>44172</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C307" s="1">
+        <v>30300131095</v>
+      </c>
+      <c r="D307" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A308" s="5"/>
+      <c r="B308" s="1"/>
+      <c r="C308" s="1"/>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A309" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B309" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C309" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D309" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A310" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C310" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D310" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A311" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B311" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C311" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D311" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A312" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B312" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C312" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D312" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A313" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B313" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C313" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D313" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A314" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B314" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C314" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D314" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A315" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C315" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D315" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A316" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B316" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C316" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D316" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A317" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C317" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D317" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A318" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B318" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C318" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D318" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A319" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C319" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D319" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A320" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B320" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C320" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D320" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A321" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C321" s="1">
+        <v>3001095</v>
+      </c>
+      <c r="D321" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A322" s="5"/>
+      <c r="B322" s="1"/>
+      <c r="C322" s="1"/>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A323" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B323" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C323" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D323" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A324" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B324" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C324" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D324" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A325" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B325" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C325" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D325" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A326" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C326" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D326" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A327" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B327" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C327" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D327" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A328" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C328" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D328" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A329" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B329" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C329" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D329" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A330" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C330" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D330" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A331" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B331" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C331" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D331" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A332" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B332" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C332" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D332" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A333" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B333" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C333" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D333" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A334" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B334" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C334" s="1">
+        <v>300131095</v>
+      </c>
+      <c r="D334" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A336" s="5">
         <v>44146</v>
       </c>
-      <c r="B307" s="1" t="s">
+      <c r="B336" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C307" s="1">
+      <c r="C336" s="1">
         <v>121795</v>
       </c>
-      <c r="D307" t="s">
+      <c r="D336" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A337" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C337" s="1">
+        <v>121795</v>
+      </c>
+      <c r="D337" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A338" s="5">
+        <v>44146</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C338" s="1">
+        <v>121795</v>
+      </c>
+      <c r="D338" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A308" s="5">
+    <row r="339" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A339" s="5">
         <v>44146</v>
       </c>
-      <c r="B308" s="1" t="s">
+      <c r="B339" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C308" s="1">
+      <c r="C339" s="1">
         <v>121795</v>
       </c>
-      <c r="D308" t="s">
+      <c r="D339" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A309" s="5">
+    <row r="340" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A340" s="5">
         <v>44146</v>
       </c>
-      <c r="B309" s="1" t="s">
+      <c r="B340" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C309" s="1">
+      <c r="C340" s="1">
         <v>121795</v>
       </c>
-      <c r="D309" t="s">
+      <c r="D340" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A310" s="5">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A341" s="5">
         <v>44146</v>
       </c>
-      <c r="B310" s="1" t="s">
+      <c r="B341" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C310" s="1">
+      <c r="C341" s="1">
         <v>121795</v>
       </c>
-      <c r="D310" t="s">
+      <c r="D341" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A311" s="5">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A342" s="5">
         <v>44146</v>
       </c>
-      <c r="B311" s="1" t="s">
+      <c r="B342" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C311" s="1">
+      <c r="C342" s="1">
         <v>121795</v>
       </c>
-      <c r="D311" t="s">
+      <c r="D342" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A312" s="5">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A343" s="5">
         <v>44146</v>
       </c>
-      <c r="B312" s="1" t="s">
+      <c r="B343" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C312" s="1">
+      <c r="C343" s="1">
         <v>121795</v>
       </c>
-      <c r="D312" t="s">
+      <c r="D343" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A313" s="5">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A344" s="5">
         <v>44146</v>
       </c>
-      <c r="B313" s="1" t="s">
+      <c r="B344" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C313" s="1">
+      <c r="C344" s="1">
         <v>121795</v>
       </c>
-      <c r="D313" t="s">
+      <c r="D344" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A315" s="5">
+    <row r="346" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A346" s="5">
         <v>44146</v>
       </c>
-      <c r="B315" s="1" t="s">
+      <c r="B346" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="C315" s="1">
+      <c r="C346" s="1">
         <v>1795</v>
       </c>
-      <c r="D315" t="s">
+      <c r="D346" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A316" s="5">
+    <row r="347" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A347" s="5">
         <v>44146</v>
       </c>
-      <c r="B316" s="1" t="s">
+      <c r="B347" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="C316" s="1">
+      <c r="C347" s="1">
         <v>1795</v>
       </c>
-      <c r="D316" t="s">
+      <c r="D347" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A317" s="5">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A348" s="5">
         <v>44146</v>
       </c>
-      <c r="B317" s="1" t="s">
+      <c r="B348" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="C317" s="1">
+      <c r="C348" s="1">
         <v>1795</v>
       </c>
-      <c r="D317" t="s">
+      <c r="D348" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A318" s="5">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A349" s="5">
         <v>44146</v>
       </c>
-      <c r="B318" s="1" t="s">
+      <c r="B349" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="C318" s="1">
+      <c r="C349" s="1">
         <v>1795</v>
       </c>
-      <c r="D318" t="s">
+      <c r="D349" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A320" s="5">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A351" s="5">
         <v>44146</v>
       </c>
-      <c r="B320" s="1" t="s">
+      <c r="B351" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C320" s="1">
+      <c r="C351" s="1">
         <v>21795</v>
       </c>
-      <c r="D320" t="s">
+      <c r="D351" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A321" s="5">
+    <row r="352" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A352" s="5">
         <v>44146</v>
       </c>
-      <c r="B321" s="1" t="s">
+      <c r="B352" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C321" s="1">
+      <c r="C352" s="1">
         <v>21795</v>
       </c>
-      <c r="D321" t="s">
+      <c r="D352" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A322" s="5">
+    <row r="353" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A353" s="5">
         <v>44146</v>
       </c>
-      <c r="B322" s="1" t="s">
+      <c r="B353" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C322" s="1">
+      <c r="C353" s="1">
         <v>21795</v>
       </c>
-      <c r="D322" t="s">
+      <c r="D353" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A324" s="5">
+    <row r="355" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A355" s="5">
         <v>44146</v>
       </c>
-      <c r="B324" s="1" t="s">
+      <c r="B355" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="C324" s="1">
+      <c r="C355" s="1">
         <v>181795</v>
       </c>
-      <c r="D324" t="s">
+      <c r="D355" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A325" s="5">
+    <row r="356" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A356" s="5">
         <v>44146</v>
       </c>
-      <c r="B325" s="1" t="s">
+      <c r="B356" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="C325" s="1">
+      <c r="C356" s="1">
         <v>181795</v>
       </c>
-      <c r="D325" t="s">
+      <c r="D356" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A326" s="5">
+    <row r="357" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A357" s="5">
         <v>44146</v>
       </c>
-      <c r="B326" s="1" t="s">
+      <c r="B357" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="C326" s="1">
+      <c r="C357" s="1">
         <v>181795</v>
       </c>
-      <c r="D326" t="s">
+      <c r="D357" t="s">
         <v>298</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Workaround for corrupted files. Log to console which folder is being read to asist troubleshooting
</commit_message>
<xml_diff>
--- a/3D networks data.xlsx
+++ b/3D networks data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nivieru\Documents\MATLAB\Maya code GUI - Niv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335F552C-5543-4A4D-BA8D-1F189FF18FF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF781DA-9DB0-436C-BA80-17B6E108DA8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19183" windowHeight="7037" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="450">
   <si>
     <t>Date</t>
   </si>
@@ -1270,6 +1270,111 @@
   </si>
   <si>
     <t>W:\phkinnerets\storage\analysis\Niv\rambam10\95%\2020_12_06 temperature\mix2 rambam10 95% sample1 25deg\Capture 5</t>
+  </si>
+  <si>
+    <t>Rambam 7 90% with 10mM Mg</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix1 Mg sample1\Capture 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix1 Mg sample1\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix1 Mg sample1\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix1 Mg sample1\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix1 Mg sample1\Capture 5</t>
+  </si>
+  <si>
+    <t>Rambam 7 90% with 10mM Mg and 300nM calyculin</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix2 calycluin + Mg sample1\Capture 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix2 calycluin + Mg sample1\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix2 calycluin + Mg sample1\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix2 calycluin + Mg sample1\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix2 calycluin + Mg sample1\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix2 calycluin + Mg sample1\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix2 calycluin + Mg sample1\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix2 calycluin + Mg sample1\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix2 calycluin + Mg sample1\Capture 9</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix2 calycluin + Mg sample1\Capture 10</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix2 calycluin + Mg sample2\Capture 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix2 calycluin + Mg sample2\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix2 calycluin + Mg sample2\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix2 calycluin + Mg sample2\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix2 calycluin + Mg sample2\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix2 calycluin + Mg sample2\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix2 calycluin + Mg sample2\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix2 calycluin + Mg sample2\Capture 8</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix2 calycluin + Mg sample2\Capture 9</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix2 calycluin + Mg sample2\Capture 10</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix1 Mg sample2\Capture 1</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix1 Mg sample2\Capture 2</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix1 Mg sample2\Capture 3</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix1 Mg sample2\Capture 4</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix1 Mg sample2\Capture 5</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix1 Mg sample2\Capture 6</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix1 Mg sample2\Capture 7</t>
+  </si>
+  <si>
+    <t>W:\phkinnerets\storage\analysis\Niv\rambam7 95%\2020_12_30 accelerations\mix1 Mg sample2\Capture 9</t>
   </si>
 </sst>
 </file>
@@ -1619,16 +1724,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BF357"/>
+  <dimension ref="A1:BF392"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A324" workbookViewId="0">
-      <selection activeCell="C291" sqref="C291"/>
+    <sheetView tabSelected="1" topLeftCell="A357" workbookViewId="0">
+      <selection activeCell="B397" sqref="B397"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="26.84375" customWidth="1"/>
-    <col min="2" max="2" width="41.15234375" customWidth="1"/>
+    <col min="2" max="2" width="48.765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.3046875" customWidth="1"/>
     <col min="4" max="4" width="61.53515625" customWidth="1"/>
   </cols>
@@ -6521,6 +6626,468 @@
         <v>298</v>
       </c>
     </row>
+    <row r="359" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A359" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B359" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C359" s="1">
+        <v>79010</v>
+      </c>
+      <c r="D359" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="360" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A360" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B360" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C360" s="1">
+        <v>79010</v>
+      </c>
+      <c r="D360" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="361" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A361" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B361" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C361" s="1">
+        <v>79010</v>
+      </c>
+      <c r="D361" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="362" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A362" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B362" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C362" s="1">
+        <v>79010</v>
+      </c>
+      <c r="D362" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="363" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A363" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B363" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C363" s="1">
+        <v>79010</v>
+      </c>
+      <c r="D363" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="364" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A364" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B364" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C364" s="1">
+        <v>79010</v>
+      </c>
+      <c r="D364" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="365" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A365" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B365" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C365" s="1">
+        <v>79010</v>
+      </c>
+      <c r="D365" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="366" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A366" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B366" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C366" s="1">
+        <v>79010</v>
+      </c>
+      <c r="D366" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="367" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A367" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B367" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C367" s="1">
+        <v>79010</v>
+      </c>
+      <c r="D367" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="368" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A368" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B368" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C368" s="1">
+        <v>79010</v>
+      </c>
+      <c r="D368" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="369" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A369" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B369" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C369" s="1">
+        <v>79010</v>
+      </c>
+      <c r="D369" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="370" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A370" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B370" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C370" s="1">
+        <v>79010</v>
+      </c>
+      <c r="D370" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="371" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A371" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B371" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C371" s="1">
+        <v>79010</v>
+      </c>
+      <c r="D371" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="373" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A373" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C373" s="1">
+        <v>79010300</v>
+      </c>
+      <c r="D373" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="374" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A374" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B374" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C374" s="1">
+        <v>79010300</v>
+      </c>
+      <c r="D374" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="375" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A375" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B375" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C375" s="1">
+        <v>79010300</v>
+      </c>
+      <c r="D375" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="376" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A376" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B376" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C376" s="1">
+        <v>-79010300</v>
+      </c>
+      <c r="D376" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="377" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A377" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B377" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C377" s="1">
+        <v>79010300</v>
+      </c>
+      <c r="D377" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="378" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A378" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B378" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C378" s="1">
+        <v>79010300</v>
+      </c>
+      <c r="D378" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="379" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A379" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B379" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C379" s="1">
+        <v>79010300</v>
+      </c>
+      <c r="D379" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="380" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A380" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B380" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C380" s="1">
+        <v>79010300</v>
+      </c>
+      <c r="D380" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="381" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A381" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B381" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C381" s="1">
+        <v>79010300</v>
+      </c>
+      <c r="D381" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="382" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A382" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B382" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C382" s="1">
+        <v>79010300</v>
+      </c>
+      <c r="D382" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="383" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A383" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B383" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C383" s="1">
+        <v>79010300</v>
+      </c>
+      <c r="D383" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="384" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A384" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B384" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C384" s="1">
+        <v>79010300</v>
+      </c>
+      <c r="D384" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="385" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A385" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B385" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C385" s="1">
+        <v>79010300</v>
+      </c>
+      <c r="D385" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="386" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A386" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B386" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C386" s="1">
+        <v>79010300</v>
+      </c>
+      <c r="D386" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="387" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A387" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B387" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C387" s="1">
+        <v>79010300</v>
+      </c>
+      <c r="D387" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="388" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A388" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B388" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C388" s="1">
+        <v>79010300</v>
+      </c>
+      <c r="D388" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="389" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A389" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B389" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C389" s="1">
+        <v>79010300</v>
+      </c>
+      <c r="D389" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A390" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B390" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C390" s="1">
+        <v>79010300</v>
+      </c>
+      <c r="D390" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A391" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B391" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C391" s="1">
+        <v>79010300</v>
+      </c>
+      <c r="D391" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="392" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A392" s="5">
+        <v>44195</v>
+      </c>
+      <c r="B392" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C392" s="1">
+        <v>79010300</v>
+      </c>
+      <c r="D392" t="s">
+        <v>441</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>